<commit_message>
Dodanie dat do kart kontroli
</commit_message>
<xml_diff>
--- a/data/wzor_00.xlsx
+++ b/data/wzor_00.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Arkusz1!$A$1:$I$40</definedName>
     <definedName name="Wybór1" localSheetId="0">Arkusz1!$B$34</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -357,7 +357,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* \-??\ _z_ł_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;____######0_);[Red]\(&quot;$&quot;____#####0\)"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,6 +605,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -667,7 +674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -984,6 +991,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2090,7 +2157,7 @@
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2194,6 +2261,41 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2284,12 +2386,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2304,6 +2400,12 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1101">
@@ -4004,22 +4106,22 @@
   </sheetPr>
   <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A24" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E37"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A23" zoomScale="115" zoomScaleNormal="70" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="8.875" customWidth="1"/>
-    <col min="4" max="4" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="8.8984375" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
+    <row r="2" spans="1:9" ht="14.4" thickBot="1">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="36.75" thickBot="1">
+    <row r="3" spans="1:9" ht="36.6" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
@@ -4049,44 +4151,44 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="48.75" customHeight="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="83">
         <v>9075</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="83">
         <v>779</v>
       </c>
-      <c r="I4" s="68" t="s">
+      <c r="I4" s="83" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="71"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4"/>
@@ -4115,7 +4217,7 @@
     <row r="14" spans="1:9">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75" thickBot="1">
+    <row r="15" spans="1:9" ht="19.8" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>3</v>
       </c>
@@ -4144,7 +4246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18">
+    <row r="16" spans="1:9" ht="19.2">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -4174,42 +4276,42 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59" t="s">
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="53" t="s">
+      <c r="H17" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="49" t="s">
+      <c r="I17" s="66" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="57"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="49"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="66"/>
     </row>
-    <row r="19" spans="1:9" ht="18">
+    <row r="19" spans="1:9" ht="19.2">
       <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
@@ -4225,145 +4327,145 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15.6">
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38" t="s">
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1">
-      <c r="A22" s="56"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
+    <row r="22" spans="1:9" ht="14.4" thickBot="1">
+      <c r="A22" s="73"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36" t="s">
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
     </row>
-    <row r="24" spans="1:9" ht="22.5">
+    <row r="24" spans="1:9" ht="20.399999999999999">
       <c r="A24" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1">
+    <row r="26" spans="1:9" ht="14.4" thickBot="1">
       <c r="A26" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40" t="s">
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52" t="s">
+      <c r="C27" s="69"/>
+      <c r="D27" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49" t="s">
+      <c r="C28" s="66"/>
+      <c r="D28" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="49" t="s">
+      <c r="C29" s="65"/>
+      <c r="D29" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" ht="22.5" customHeight="1">
       <c r="A30" s="30" t="s">
@@ -4373,31 +4475,31 @@
         <v>36</v>
       </c>
       <c r="C30" s="27"/>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
     </row>
-    <row r="31" spans="1:9" ht="22.5">
+    <row r="31" spans="1:9" ht="20.399999999999999">
       <c r="A31" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49" t="s">
+      <c r="C31" s="66"/>
+      <c r="D31" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="49"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="29" t="s">
@@ -4415,12 +4517,12 @@
       <c r="E32" s="14">
         <v>2.5</v>
       </c>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -4428,107 +4530,107 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
+    <row r="34" spans="1:9" ht="14.4" thickBot="1">
       <c r="A34" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44" t="s">
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
     </row>
     <row r="35" spans="1:9" ht="26.25" customHeight="1" thickBot="1">
       <c r="A35" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1">
-      <c r="A36" s="67" t="s">
+      <c r="A36" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62" t="s">
+      <c r="B36" s="79"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="63"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="80"/>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61" t="s">
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="64"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="81"/>
     </row>
     <row r="38" spans="1:9" ht="27" customHeight="1">
-      <c r="A38" s="65"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="45"/>
     </row>
     <row r="39" spans="1:9" ht="27" customHeight="1">
-      <c r="A39" s="66"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="48"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1">
-      <c r="A40" s="66"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
+      <c r="A40" s="87"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="50"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75">
+    <row r="42" spans="1:9" ht="15.6">
       <c r="A42" s="13"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -4536,7 +4638,11 @@
       <c r="E42" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="47">
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="A36:E36"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
@@ -4546,12 +4652,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I40"/>
-    <mergeCell ref="A38:E40"/>
-    <mergeCell ref="A36:E36"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="A21:A22"/>
@@ -4613,7 +4713,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nowe funkcje: Dodanie tabeli z wymiarami elemntów łożysk. Dodanie funkcjonalności eksportujących wymiary łożysk do kart kontroli.
</commit_message>
<xml_diff>
--- a/data/wzor_00.xlsx
+++ b/data/wzor_00.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.wawrzyniak\Documents\NetBeansProjects\material-manager\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561B7CFA-424A-4752-A075-B0889902AC58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27810" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Arkusz1!$A$1:$I$40</definedName>
     <definedName name="Wybór1" localSheetId="0">Arkusz1!$B$34</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -22,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -350,12 +357,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* \-??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;____######0_);[Red]\(&quot;$&quot;____#####0\)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* \-??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;____######0_);[Red]\(&quot;$&quot;____#####0\)"/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1057,104 +1064,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1205,81 +1212,81 @@
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
@@ -1291,7 +1298,7 @@
     <xf numFmtId="38" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
@@ -2296,1220 +2303,1220 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1101">
-    <cellStyle name="_PERSONAL" xfId="2"/>
-    <cellStyle name="_PERSONAL_1" xfId="3"/>
-    <cellStyle name="Comma 2" xfId="4"/>
-    <cellStyle name="Comma 2 2" xfId="5"/>
-    <cellStyle name="Comma 2 2 2" xfId="6"/>
-    <cellStyle name="Comma 2 3" xfId="7"/>
-    <cellStyle name="Comma 2 3 2" xfId="8"/>
-    <cellStyle name="Comma 2 3 2 2" xfId="9"/>
-    <cellStyle name="Comma 2 3 2 2 2" xfId="10"/>
-    <cellStyle name="Comma 2 3 2 2 2 2" xfId="11"/>
-    <cellStyle name="Comma 2 3 2 2 3" xfId="12"/>
-    <cellStyle name="Comma 2 3 2 3" xfId="13"/>
-    <cellStyle name="Comma 2 3 2 3 2" xfId="14"/>
-    <cellStyle name="Comma 2 3 2 4" xfId="15"/>
-    <cellStyle name="Comma 2 3 3" xfId="16"/>
-    <cellStyle name="Comma 2 3 3 2" xfId="17"/>
-    <cellStyle name="Comma 2 3 3 2 2" xfId="18"/>
-    <cellStyle name="Comma 2 3 3 3" xfId="19"/>
-    <cellStyle name="Comma 2 3 4" xfId="20"/>
-    <cellStyle name="Comma 2 3 4 2" xfId="21"/>
-    <cellStyle name="Comma 2 3 5" xfId="22"/>
-    <cellStyle name="Comma 2 4" xfId="23"/>
-    <cellStyle name="Comma 2 4 2" xfId="24"/>
-    <cellStyle name="Comma 2 4 2 2" xfId="25"/>
-    <cellStyle name="Comma 2 4 2 2 2" xfId="26"/>
-    <cellStyle name="Comma 2 4 2 2 2 2" xfId="27"/>
-    <cellStyle name="Comma 2 4 2 2 3" xfId="28"/>
-    <cellStyle name="Comma 2 4 2 3" xfId="29"/>
-    <cellStyle name="Comma 2 4 2 3 2" xfId="30"/>
-    <cellStyle name="Comma 2 4 2 4" xfId="31"/>
-    <cellStyle name="Comma 2 4 3" xfId="32"/>
-    <cellStyle name="Comma 2 4 3 2" xfId="33"/>
-    <cellStyle name="Comma 2 4 3 2 2" xfId="34"/>
-    <cellStyle name="Comma 2 4 3 3" xfId="35"/>
-    <cellStyle name="Comma 2 4 4" xfId="36"/>
-    <cellStyle name="Comma 2 4 4 2" xfId="37"/>
-    <cellStyle name="Comma 2 4 5" xfId="38"/>
-    <cellStyle name="Comma 2 5" xfId="39"/>
-    <cellStyle name="Comma 2 5 2" xfId="40"/>
-    <cellStyle name="Comma 2 5 2 2" xfId="41"/>
-    <cellStyle name="Comma 2 5 2 2 2" xfId="42"/>
-    <cellStyle name="Comma 2 5 2 3" xfId="43"/>
-    <cellStyle name="Comma 2 5 3" xfId="44"/>
-    <cellStyle name="Comma 2 5 3 2" xfId="45"/>
-    <cellStyle name="Comma 2 5 4" xfId="46"/>
-    <cellStyle name="Comma 2 6" xfId="47"/>
-    <cellStyle name="Comma 2 6 2" xfId="48"/>
-    <cellStyle name="Comma 2 6 2 2" xfId="49"/>
-    <cellStyle name="Comma 2 6 3" xfId="50"/>
-    <cellStyle name="Comma 2 7" xfId="51"/>
-    <cellStyle name="Comma 2 7 2" xfId="52"/>
-    <cellStyle name="Comma 2 8" xfId="53"/>
-    <cellStyle name="Comma 3" xfId="54"/>
-    <cellStyle name="Comma 3 2" xfId="55"/>
-    <cellStyle name="Comma 3 2 2" xfId="56"/>
-    <cellStyle name="Comma 3 2 2 2" xfId="57"/>
-    <cellStyle name="Comma 3 2 2 2 2" xfId="58"/>
-    <cellStyle name="Comma 3 2 2 2 2 2" xfId="59"/>
-    <cellStyle name="Comma 3 2 2 2 3" xfId="60"/>
-    <cellStyle name="Comma 3 2 2 3" xfId="61"/>
-    <cellStyle name="Comma 3 2 2 3 2" xfId="62"/>
-    <cellStyle name="Comma 3 2 2 4" xfId="63"/>
-    <cellStyle name="Comma 3 2 3" xfId="64"/>
-    <cellStyle name="Comma 3 2 3 2" xfId="65"/>
-    <cellStyle name="Comma 3 2 3 2 2" xfId="66"/>
-    <cellStyle name="Comma 3 2 3 3" xfId="67"/>
-    <cellStyle name="Comma 3 2 4" xfId="68"/>
-    <cellStyle name="Comma 3 2 4 2" xfId="69"/>
-    <cellStyle name="Comma 3 2 5" xfId="70"/>
-    <cellStyle name="Comma 3 3" xfId="71"/>
-    <cellStyle name="Comma 3 3 2" xfId="72"/>
-    <cellStyle name="Comma 3 3 2 2" xfId="73"/>
-    <cellStyle name="Comma 3 3 2 2 2" xfId="74"/>
-    <cellStyle name="Comma 3 3 2 2 2 2" xfId="75"/>
-    <cellStyle name="Comma 3 3 2 2 3" xfId="76"/>
-    <cellStyle name="Comma 3 3 2 3" xfId="77"/>
-    <cellStyle name="Comma 3 3 2 3 2" xfId="78"/>
-    <cellStyle name="Comma 3 3 2 4" xfId="79"/>
-    <cellStyle name="Comma 3 3 3" xfId="80"/>
-    <cellStyle name="Comma 3 3 3 2" xfId="81"/>
-    <cellStyle name="Comma 3 3 3 2 2" xfId="82"/>
-    <cellStyle name="Comma 3 3 3 3" xfId="83"/>
-    <cellStyle name="Comma 3 3 4" xfId="84"/>
-    <cellStyle name="Comma 3 3 4 2" xfId="85"/>
-    <cellStyle name="Comma 3 3 5" xfId="86"/>
-    <cellStyle name="Comma 3 4" xfId="87"/>
-    <cellStyle name="Comma 3 4 2" xfId="88"/>
-    <cellStyle name="Comma 3 4 2 2" xfId="89"/>
-    <cellStyle name="Comma 3 4 2 2 2" xfId="90"/>
-    <cellStyle name="Comma 3 4 2 3" xfId="91"/>
-    <cellStyle name="Comma 3 4 3" xfId="92"/>
-    <cellStyle name="Comma 3 4 3 2" xfId="93"/>
-    <cellStyle name="Comma 3 4 4" xfId="94"/>
-    <cellStyle name="Comma 3 5" xfId="95"/>
-    <cellStyle name="Comma 3 5 2" xfId="96"/>
-    <cellStyle name="Comma 3 5 2 2" xfId="97"/>
-    <cellStyle name="Comma 3 5 3" xfId="98"/>
-    <cellStyle name="Comma 3 6" xfId="99"/>
-    <cellStyle name="Comma 3 6 2" xfId="100"/>
-    <cellStyle name="Comma 3 7" xfId="101"/>
-    <cellStyle name="Currency 2" xfId="102"/>
-    <cellStyle name="Currency 2 2" xfId="103"/>
-    <cellStyle name="Currency 2 2 2" xfId="104"/>
-    <cellStyle name="Currency 2 2 2 2" xfId="105"/>
-    <cellStyle name="Currency 2 2 2 2 2" xfId="106"/>
-    <cellStyle name="Currency 2 2 2 2 2 2" xfId="107"/>
-    <cellStyle name="Currency 2 2 2 2 2 2 2" xfId="108"/>
-    <cellStyle name="Currency 2 2 2 2 2 3" xfId="109"/>
-    <cellStyle name="Currency 2 2 2 2 3" xfId="110"/>
-    <cellStyle name="Currency 2 2 2 2 3 2" xfId="111"/>
-    <cellStyle name="Currency 2 2 2 2 4" xfId="112"/>
-    <cellStyle name="Currency 2 2 2 3" xfId="113"/>
-    <cellStyle name="Currency 2 2 2 3 2" xfId="114"/>
-    <cellStyle name="Currency 2 2 2 3 2 2" xfId="115"/>
-    <cellStyle name="Currency 2 2 2 3 3" xfId="116"/>
-    <cellStyle name="Currency 2 2 2 4" xfId="117"/>
-    <cellStyle name="Currency 2 2 2 4 2" xfId="118"/>
-    <cellStyle name="Currency 2 2 2 5" xfId="119"/>
-    <cellStyle name="Currency 2 2 3" xfId="120"/>
-    <cellStyle name="Currency 2 2 3 2" xfId="121"/>
-    <cellStyle name="Currency 2 2 3 2 2" xfId="122"/>
-    <cellStyle name="Currency 2 2 3 2 2 2" xfId="123"/>
-    <cellStyle name="Currency 2 2 3 2 2 2 2" xfId="124"/>
-    <cellStyle name="Currency 2 2 3 2 2 3" xfId="125"/>
-    <cellStyle name="Currency 2 2 3 2 3" xfId="126"/>
-    <cellStyle name="Currency 2 2 3 2 3 2" xfId="127"/>
-    <cellStyle name="Currency 2 2 3 2 4" xfId="128"/>
-    <cellStyle name="Currency 2 2 3 3" xfId="129"/>
-    <cellStyle name="Currency 2 2 3 3 2" xfId="130"/>
-    <cellStyle name="Currency 2 2 3 3 2 2" xfId="131"/>
-    <cellStyle name="Currency 2 2 3 3 3" xfId="132"/>
-    <cellStyle name="Currency 2 2 3 4" xfId="133"/>
-    <cellStyle name="Currency 2 2 3 4 2" xfId="134"/>
-    <cellStyle name="Currency 2 2 3 5" xfId="135"/>
-    <cellStyle name="Currency 2 2 4" xfId="136"/>
-    <cellStyle name="Currency 2 2 4 2" xfId="137"/>
-    <cellStyle name="Currency 2 2 4 2 2" xfId="138"/>
-    <cellStyle name="Currency 2 2 4 2 2 2" xfId="139"/>
-    <cellStyle name="Currency 2 2 4 2 3" xfId="140"/>
-    <cellStyle name="Currency 2 2 4 3" xfId="141"/>
-    <cellStyle name="Currency 2 2 4 3 2" xfId="142"/>
-    <cellStyle name="Currency 2 2 4 4" xfId="143"/>
-    <cellStyle name="Currency 2 2 5" xfId="144"/>
-    <cellStyle name="Currency 2 2 5 2" xfId="145"/>
-    <cellStyle name="Currency 2 2 5 2 2" xfId="146"/>
-    <cellStyle name="Currency 2 2 5 3" xfId="147"/>
-    <cellStyle name="Currency 2 2 6" xfId="148"/>
-    <cellStyle name="Currency 2 2 6 2" xfId="149"/>
-    <cellStyle name="Currency 2 2 7" xfId="150"/>
-    <cellStyle name="Currency 2 3" xfId="151"/>
-    <cellStyle name="Dziesiętny 10" xfId="152"/>
-    <cellStyle name="Dziesiętny 2" xfId="153"/>
-    <cellStyle name="Dziesiętny 2 2" xfId="154"/>
-    <cellStyle name="Dziesiętny 2 2 2" xfId="155"/>
-    <cellStyle name="Dziesiętny 2 3" xfId="156"/>
-    <cellStyle name="Dziesiętny 2 3 2" xfId="157"/>
-    <cellStyle name="Dziesiętny 2 3 2 2" xfId="158"/>
-    <cellStyle name="Dziesiętny 2 4" xfId="159"/>
-    <cellStyle name="Dziesiętny 2 5" xfId="160"/>
-    <cellStyle name="Dziesiętny 3" xfId="161"/>
-    <cellStyle name="Dziesiętny 3 2" xfId="162"/>
-    <cellStyle name="Dziesiętny 4" xfId="163"/>
-    <cellStyle name="Dziesiętny 4 2" xfId="164"/>
-    <cellStyle name="Dziesiętny 4 2 2" xfId="165"/>
-    <cellStyle name="Dziesiętny 4 2 2 2" xfId="166"/>
-    <cellStyle name="Dziesiętny 4 2 2 2 2" xfId="167"/>
-    <cellStyle name="Dziesiętny 4 2 2 2 2 2" xfId="168"/>
-    <cellStyle name="Dziesiętny 4 2 2 2 3" xfId="169"/>
-    <cellStyle name="Dziesiętny 4 2 2 3" xfId="170"/>
-    <cellStyle name="Dziesiętny 4 2 2 3 2" xfId="171"/>
-    <cellStyle name="Dziesiętny 4 2 2 4" xfId="172"/>
-    <cellStyle name="Dziesiętny 4 2 3" xfId="173"/>
-    <cellStyle name="Dziesiętny 4 2 3 2" xfId="174"/>
-    <cellStyle name="Dziesiętny 4 2 3 2 2" xfId="175"/>
-    <cellStyle name="Dziesiętny 4 2 3 3" xfId="176"/>
-    <cellStyle name="Dziesiętny 4 2 4" xfId="177"/>
-    <cellStyle name="Dziesiętny 4 2 4 2" xfId="178"/>
-    <cellStyle name="Dziesiętny 4 2 5" xfId="179"/>
-    <cellStyle name="Dziesiętny 4 3" xfId="180"/>
-    <cellStyle name="Dziesiętny 4 3 2" xfId="181"/>
-    <cellStyle name="Dziesiętny 4 3 2 2" xfId="182"/>
-    <cellStyle name="Dziesiętny 4 3 2 2 2" xfId="183"/>
-    <cellStyle name="Dziesiętny 4 3 2 2 2 2" xfId="184"/>
-    <cellStyle name="Dziesiętny 4 3 2 2 3" xfId="185"/>
-    <cellStyle name="Dziesiętny 4 3 2 3" xfId="186"/>
-    <cellStyle name="Dziesiętny 4 3 2 3 2" xfId="187"/>
-    <cellStyle name="Dziesiętny 4 3 2 4" xfId="188"/>
-    <cellStyle name="Dziesiętny 4 3 3" xfId="189"/>
-    <cellStyle name="Dziesiętny 4 3 3 2" xfId="190"/>
-    <cellStyle name="Dziesiętny 4 3 3 2 2" xfId="191"/>
-    <cellStyle name="Dziesiętny 4 3 3 3" xfId="192"/>
-    <cellStyle name="Dziesiętny 4 3 4" xfId="193"/>
-    <cellStyle name="Dziesiętny 4 3 4 2" xfId="194"/>
-    <cellStyle name="Dziesiętny 4 3 5" xfId="195"/>
-    <cellStyle name="Dziesiętny 4 4" xfId="196"/>
-    <cellStyle name="Dziesiętny 4 4 2" xfId="197"/>
-    <cellStyle name="Dziesiętny 4 4 2 2" xfId="198"/>
-    <cellStyle name="Dziesiętny 4 4 2 2 2" xfId="199"/>
-    <cellStyle name="Dziesiętny 4 4 2 3" xfId="200"/>
-    <cellStyle name="Dziesiętny 4 4 3" xfId="201"/>
-    <cellStyle name="Dziesiętny 4 4 3 2" xfId="202"/>
-    <cellStyle name="Dziesiętny 4 4 4" xfId="203"/>
-    <cellStyle name="Dziesiętny 4 5" xfId="204"/>
-    <cellStyle name="Dziesiętny 4 5 2" xfId="205"/>
-    <cellStyle name="Dziesiętny 4 5 2 2" xfId="206"/>
-    <cellStyle name="Dziesiętny 4 5 3" xfId="207"/>
-    <cellStyle name="Dziesiętny 4 6" xfId="208"/>
-    <cellStyle name="Dziesiętny 4 6 2" xfId="209"/>
-    <cellStyle name="Dziesiętny 4 7" xfId="210"/>
-    <cellStyle name="Dziesiętny 5" xfId="211"/>
-    <cellStyle name="Dziesiętny 5 2" xfId="212"/>
-    <cellStyle name="Dziesiętny 5 3" xfId="213"/>
-    <cellStyle name="Dziesiętny 5 3 2" xfId="214"/>
-    <cellStyle name="Dziesiętny 5 3 2 2" xfId="215"/>
-    <cellStyle name="Dziesiętny 5 3 3" xfId="216"/>
-    <cellStyle name="Dziesiętny 5 4" xfId="217"/>
-    <cellStyle name="Dziesiętny 5 4 2" xfId="218"/>
-    <cellStyle name="Dziesiętny 5 5" xfId="219"/>
-    <cellStyle name="Dziesiętny 6" xfId="220"/>
-    <cellStyle name="Dziesiętny 7" xfId="221"/>
-    <cellStyle name="Dziesiętny 7 2" xfId="222"/>
-    <cellStyle name="Dziesiętny 7 2 2" xfId="223"/>
-    <cellStyle name="Dziesiętny 7 3" xfId="224"/>
-    <cellStyle name="Dziesiętny 8" xfId="225"/>
-    <cellStyle name="Dziesiętny 9" xfId="226"/>
-    <cellStyle name="Excel Built-in 20% - Accent1" xfId="227"/>
-    <cellStyle name="Excel Built-in 60% - Accent1" xfId="228"/>
-    <cellStyle name="Excel Built-in Bad" xfId="229"/>
-    <cellStyle name="Excel Built-in Good" xfId="230"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="231"/>
-    <cellStyle name="Excel Built-in Normal" xfId="232"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="233"/>
-    <cellStyle name="Excel Built-in Normal 2 2" xfId="234"/>
-    <cellStyle name="Grey" xfId="235"/>
-    <cellStyle name="Input [yellow]" xfId="236"/>
-    <cellStyle name="None" xfId="237"/>
-    <cellStyle name="Normal - Style1" xfId="238"/>
-    <cellStyle name="Normal 2" xfId="239"/>
-    <cellStyle name="Normal 2 2" xfId="240"/>
-    <cellStyle name="Normal 3" xfId="241"/>
-    <cellStyle name="Normal 3 2" xfId="242"/>
-    <cellStyle name="Normal 3 2 2" xfId="243"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="244"/>
-    <cellStyle name="Normal 3 2 2 2 2" xfId="245"/>
-    <cellStyle name="Normal 3 2 2 2 2 2" xfId="246"/>
-    <cellStyle name="Normal 3 2 2 2 2 2 2" xfId="247"/>
-    <cellStyle name="Normal 3 2 2 2 2 3" xfId="248"/>
-    <cellStyle name="Normal 3 2 2 2 3" xfId="249"/>
-    <cellStyle name="Normal 3 2 2 2 3 2" xfId="250"/>
-    <cellStyle name="Normal 3 2 2 2 4" xfId="251"/>
-    <cellStyle name="Normal 3 2 2 3" xfId="252"/>
-    <cellStyle name="Normal 3 2 2 3 2" xfId="253"/>
-    <cellStyle name="Normal 3 2 2 3 2 2" xfId="254"/>
-    <cellStyle name="Normal 3 2 2 3 3" xfId="255"/>
-    <cellStyle name="Normal 3 2 2 4" xfId="256"/>
-    <cellStyle name="Normal 3 2 2 4 2" xfId="257"/>
-    <cellStyle name="Normal 3 2 2 5" xfId="258"/>
-    <cellStyle name="Normal 3 2 3" xfId="259"/>
-    <cellStyle name="Normal 3 2 3 2" xfId="260"/>
-    <cellStyle name="Normal 3 2 3 2 2" xfId="261"/>
-    <cellStyle name="Normal 3 2 3 2 2 2" xfId="262"/>
-    <cellStyle name="Normal 3 2 3 2 2 2 2" xfId="263"/>
-    <cellStyle name="Normal 3 2 3 2 2 3" xfId="264"/>
-    <cellStyle name="Normal 3 2 3 2 3" xfId="265"/>
-    <cellStyle name="Normal 3 2 3 2 3 2" xfId="266"/>
-    <cellStyle name="Normal 3 2 3 2 4" xfId="267"/>
-    <cellStyle name="Normal 3 2 3 3" xfId="268"/>
-    <cellStyle name="Normal 3 2 3 3 2" xfId="269"/>
-    <cellStyle name="Normal 3 2 3 3 2 2" xfId="270"/>
-    <cellStyle name="Normal 3 2 3 3 3" xfId="271"/>
-    <cellStyle name="Normal 3 2 3 4" xfId="272"/>
-    <cellStyle name="Normal 3 2 3 4 2" xfId="273"/>
-    <cellStyle name="Normal 3 2 3 5" xfId="274"/>
-    <cellStyle name="Normal 3 2 4" xfId="275"/>
-    <cellStyle name="Normal 3 2 4 2" xfId="276"/>
-    <cellStyle name="Normal 3 2 4 2 2" xfId="277"/>
-    <cellStyle name="Normal 3 2 4 2 2 2" xfId="278"/>
-    <cellStyle name="Normal 3 2 4 2 3" xfId="279"/>
-    <cellStyle name="Normal 3 2 4 3" xfId="280"/>
-    <cellStyle name="Normal 3 2 4 3 2" xfId="281"/>
-    <cellStyle name="Normal 3 2 4 4" xfId="282"/>
-    <cellStyle name="Normal 3 2 5" xfId="283"/>
-    <cellStyle name="Normal 3 2 5 2" xfId="284"/>
-    <cellStyle name="Normal 3 2 5 2 2" xfId="285"/>
-    <cellStyle name="Normal 3 2 5 3" xfId="286"/>
-    <cellStyle name="Normal 3 2 6" xfId="287"/>
-    <cellStyle name="Normal 3 2 6 2" xfId="288"/>
-    <cellStyle name="Normal 3 2 7" xfId="289"/>
-    <cellStyle name="Normal 3 3" xfId="290"/>
-    <cellStyle name="Normal 3 3 2" xfId="291"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="292"/>
-    <cellStyle name="Normal 3 3 2 2 2" xfId="293"/>
-    <cellStyle name="Normal 3 3 2 2 2 2" xfId="294"/>
-    <cellStyle name="Normal 3 3 2 2 3" xfId="295"/>
-    <cellStyle name="Normal 3 3 2 3" xfId="296"/>
-    <cellStyle name="Normal 3 3 2 3 2" xfId="297"/>
-    <cellStyle name="Normal 3 3 2 4" xfId="298"/>
-    <cellStyle name="Normal 3 3 3" xfId="299"/>
-    <cellStyle name="Normal 3 3 3 2" xfId="300"/>
-    <cellStyle name="Normal 3 3 3 2 2" xfId="301"/>
-    <cellStyle name="Normal 3 3 3 3" xfId="302"/>
-    <cellStyle name="Normal 3 3 4" xfId="303"/>
-    <cellStyle name="Normal 3 3 4 2" xfId="304"/>
-    <cellStyle name="Normal 3 3 5" xfId="305"/>
-    <cellStyle name="Normal 3 4" xfId="306"/>
-    <cellStyle name="Normal 3 4 2" xfId="307"/>
-    <cellStyle name="Normal 3 4 2 2" xfId="308"/>
-    <cellStyle name="Normal 3 4 2 2 2" xfId="309"/>
-    <cellStyle name="Normal 3 4 2 2 2 2" xfId="310"/>
-    <cellStyle name="Normal 3 4 2 2 3" xfId="311"/>
-    <cellStyle name="Normal 3 4 2 3" xfId="312"/>
-    <cellStyle name="Normal 3 4 2 3 2" xfId="313"/>
-    <cellStyle name="Normal 3 4 2 4" xfId="314"/>
-    <cellStyle name="Normal 3 4 3" xfId="315"/>
-    <cellStyle name="Normal 3 4 3 2" xfId="316"/>
-    <cellStyle name="Normal 3 4 3 2 2" xfId="317"/>
-    <cellStyle name="Normal 3 4 3 3" xfId="318"/>
-    <cellStyle name="Normal 3 4 4" xfId="319"/>
-    <cellStyle name="Normal 3 4 4 2" xfId="320"/>
-    <cellStyle name="Normal 3 4 5" xfId="321"/>
-    <cellStyle name="Normal 3 5" xfId="322"/>
-    <cellStyle name="Normal 3 5 2" xfId="323"/>
-    <cellStyle name="Normal 3 5 2 2" xfId="324"/>
-    <cellStyle name="Normal 3 5 2 2 2" xfId="325"/>
-    <cellStyle name="Normal 3 5 2 3" xfId="326"/>
-    <cellStyle name="Normal 3 5 3" xfId="327"/>
-    <cellStyle name="Normal 3 5 3 2" xfId="328"/>
-    <cellStyle name="Normal 3 5 4" xfId="329"/>
-    <cellStyle name="Normal 3 6" xfId="330"/>
-    <cellStyle name="Normal 3 6 2" xfId="331"/>
-    <cellStyle name="Normal 3 6 2 2" xfId="332"/>
-    <cellStyle name="Normal 3 6 3" xfId="333"/>
-    <cellStyle name="Normal 3 7" xfId="334"/>
-    <cellStyle name="Normal 3 7 2" xfId="335"/>
-    <cellStyle name="Normal 3 8" xfId="336"/>
-    <cellStyle name="Normal 4" xfId="337"/>
-    <cellStyle name="normální_laroux" xfId="338"/>
+    <cellStyle name="_PERSONAL" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="_PERSONAL_1" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 2 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 3 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 2 3 2 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 2 3 2 2 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Comma 2 3 2 2 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Comma 2 3 2 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Comma 2 3 2 3 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Comma 2 3 2 4" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Comma 2 3 3" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Comma 2 3 3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Comma 2 3 3 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Comma 2 3 3 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Comma 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Comma 2 3 4 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Comma 2 3 5" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Comma 2 4" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Comma 2 4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Comma 2 4 2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Comma 2 4 2 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Comma 2 4 2 2 2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Comma 2 4 2 2 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Comma 2 4 2 3" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Comma 2 4 2 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Comma 2 4 2 4" xfId="31" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Comma 2 4 3" xfId="32" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Comma 2 4 3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 2 4 3 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 2 4 3 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 2 4 4" xfId="36" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 2 4 4 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 2 4 5" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 2 5" xfId="39" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Comma 2 5 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Comma 2 5 2 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Comma 2 5 2 2 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Comma 2 5 2 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Comma 2 5 3" xfId="44" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Comma 2 5 3 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Comma 2 5 4" xfId="46" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Comma 2 6" xfId="47" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Comma 2 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Comma 2 6 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Comma 2 6 3" xfId="50" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Comma 2 7" xfId="51" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Comma 2 7 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Comma 2 8" xfId="53" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Comma 3" xfId="54" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Comma 3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Comma 3 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Comma 3 2 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Comma 3 2 2 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Comma 3 2 2 2 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Comma 3 2 2 2 3" xfId="60" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Comma 3 2 2 3" xfId="61" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Comma 3 2 2 3 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Comma 3 2 2 4" xfId="63" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Comma 3 2 3" xfId="64" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Comma 3 2 3 2" xfId="65" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Comma 3 2 3 2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Comma 3 2 3 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Comma 3 2 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Comma 3 2 4 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Comma 3 2 5" xfId="70" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Comma 3 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Comma 3 3 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Comma 3 3 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Comma 3 3 2 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Comma 3 3 2 2 2 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Comma 3 3 2 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Comma 3 3 2 3" xfId="77" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Comma 3 3 2 3 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Comma 3 3 2 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Comma 3 3 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Comma 3 3 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Comma 3 3 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Comma 3 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Comma 3 3 4" xfId="84" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Comma 3 3 4 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Comma 3 3 5" xfId="86" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Comma 3 4" xfId="87" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Comma 3 4 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Comma 3 4 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Comma 3 4 2 2 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Comma 3 4 2 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Comma 3 4 3" xfId="92" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Comma 3 4 3 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Comma 3 4 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Comma 3 5" xfId="95" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Comma 3 5 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Comma 3 5 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Comma 3 5 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Comma 3 6" xfId="99" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Comma 3 6 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Comma 3 7" xfId="101" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Currency 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Currency 2 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Currency 2 2 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Currency 2 2 2 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Currency 2 2 2 2 2" xfId="106" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Currency 2 2 2 2 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Currency 2 2 2 2 2 2 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Currency 2 2 2 2 2 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Currency 2 2 2 2 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Currency 2 2 2 2 3 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Currency 2 2 2 2 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Currency 2 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Currency 2 2 2 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Currency 2 2 2 3 2 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Currency 2 2 2 3 3" xfId="116" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Currency 2 2 2 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Currency 2 2 2 4 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Currency 2 2 2 5" xfId="119" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Currency 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Currency 2 2 3 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Currency 2 2 3 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Currency 2 2 3 2 2 2" xfId="123" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Currency 2 2 3 2 2 2 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Currency 2 2 3 2 2 3" xfId="125" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Currency 2 2 3 2 3" xfId="126" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Currency 2 2 3 2 3 2" xfId="127" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Currency 2 2 3 2 4" xfId="128" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Currency 2 2 3 3" xfId="129" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Currency 2 2 3 3 2" xfId="130" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Currency 2 2 3 3 2 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Currency 2 2 3 3 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Currency 2 2 3 4" xfId="133" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Currency 2 2 3 4 2" xfId="134" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Currency 2 2 3 5" xfId="135" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Currency 2 2 4" xfId="136" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Currency 2 2 4 2" xfId="137" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Currency 2 2 4 2 2" xfId="138" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Currency 2 2 4 2 2 2" xfId="139" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Currency 2 2 4 2 3" xfId="140" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Currency 2 2 4 3" xfId="141" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Currency 2 2 4 3 2" xfId="142" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Currency 2 2 4 4" xfId="143" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Currency 2 2 5" xfId="144" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Currency 2 2 5 2" xfId="145" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Currency 2 2 5 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Currency 2 2 5 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Currency 2 2 6" xfId="148" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Currency 2 2 6 2" xfId="149" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Currency 2 2 7" xfId="150" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Currency 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Dziesiętny 10" xfId="152" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Dziesiętny 2" xfId="153" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Dziesiętny 2 2" xfId="154" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Dziesiętny 2 2 2" xfId="155" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Dziesiętny 2 3" xfId="156" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Dziesiętny 2 3 2" xfId="157" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Dziesiętny 2 3 2 2" xfId="158" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Dziesiętny 2 4" xfId="159" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Dziesiętny 2 5" xfId="160" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Dziesiętny 3" xfId="161" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Dziesiętny 3 2" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Dziesiętny 4" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Dziesiętny 4 2" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 2" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 2 2" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 2 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 2 3" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 3" xfId="170" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 3 2" xfId="171" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Dziesiętny 4 2 2 4" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Dziesiętny 4 2 3" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Dziesiętny 4 2 3 2" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Dziesiętny 4 2 3 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Dziesiętny 4 2 3 3" xfId="176" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Dziesiętny 4 2 4" xfId="177" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Dziesiętny 4 2 4 2" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Dziesiętny 4 2 5" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Dziesiętny 4 3" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 2 2" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 2 2 2" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 2 3" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 3 2" xfId="187" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Dziesiętny 4 3 2 4" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Dziesiętny 4 3 3" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Dziesiętny 4 3 3 2" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Dziesiętny 4 3 3 2 2" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Dziesiętny 4 3 3 3" xfId="192" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Dziesiętny 4 3 4" xfId="193" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Dziesiętny 4 3 4 2" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Dziesiętny 4 3 5" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Dziesiętny 4 4" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Dziesiętny 4 4 2" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Dziesiętny 4 4 2 2" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Dziesiętny 4 4 2 2 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Dziesiętny 4 4 2 3" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Dziesiętny 4 4 3" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Dziesiętny 4 4 3 2" xfId="202" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Dziesiętny 4 4 4" xfId="203" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Dziesiętny 4 5" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Dziesiętny 4 5 2" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Dziesiętny 4 5 2 2" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Dziesiętny 4 5 3" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Dziesiętny 4 6" xfId="208" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Dziesiętny 4 6 2" xfId="209" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Dziesiętny 4 7" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Dziesiętny 5" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Dziesiętny 5 2" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Dziesiętny 5 3" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Dziesiętny 5 3 2" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Dziesiętny 5 3 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Dziesiętny 5 3 3" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Dziesiętny 5 4" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Dziesiętny 5 4 2" xfId="218" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Dziesiętny 5 5" xfId="219" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Dziesiętny 6" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Dziesiętny 7" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Dziesiętny 7 2" xfId="222" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Dziesiętny 7 2 2" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Dziesiętny 7 3" xfId="224" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Dziesiętny 8" xfId="225" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Dziesiętny 9" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Excel Built-in 20% - Accent1" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Excel Built-in 60% - Accent1" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Excel Built-in Bad" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Excel Built-in Good" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="232" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Excel Built-in Normal 2 2" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Grey" xfId="235" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Input [yellow]" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="None" xfId="237" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Normal - Style1" xfId="238" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 2" xfId="239" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Normal 2 2" xfId="240" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Normal 3" xfId="241" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Normal 3 2" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Normal 3 2 2 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Normal 3 2 2 2 2 2" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Normal 3 2 2 2 2 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Normal 3 2 2 2 2 3" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Normal 3 2 2 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Normal 3 2 2 2 3 2" xfId="250" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Normal 3 2 2 2 4" xfId="251" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Normal 3 2 2 3" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Normal 3 2 2 3 2" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Normal 3 2 2 3 2 2" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Normal 3 2 2 3 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Normal 3 2 2 4" xfId="256" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Normal 3 2 2 4 2" xfId="257" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Normal 3 2 2 5" xfId="258" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Normal 3 2 3 2" xfId="260" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Normal 3 2 3 2 2" xfId="261" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Normal 3 2 3 2 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Normal 3 2 3 2 2 2 2" xfId="263" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Normal 3 2 3 2 2 3" xfId="264" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Normal 3 2 3 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Normal 3 2 3 2 3 2" xfId="266" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Normal 3 2 3 2 4" xfId="267" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Normal 3 2 3 3" xfId="268" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Normal 3 2 3 3 2" xfId="269" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Normal 3 2 3 3 2 2" xfId="270" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Normal 3 2 3 3 3" xfId="271" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Normal 3 2 3 4" xfId="272" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Normal 3 2 3 4 2" xfId="273" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Normal 3 2 3 5" xfId="274" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Normal 3 2 4" xfId="275" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Normal 3 2 4 2" xfId="276" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 3 2 4 2 2" xfId="277" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Normal 3 2 4 2 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Normal 3 2 4 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Normal 3 2 4 3" xfId="280" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Normal 3 2 4 3 2" xfId="281" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Normal 3 2 4 4" xfId="282" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Normal 3 2 5" xfId="283" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Normal 3 2 5 2" xfId="284" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Normal 3 2 5 2 2" xfId="285" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Normal 3 2 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Normal 3 2 6" xfId="287" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Normal 3 2 6 2" xfId="288" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Normal 3 2 7" xfId="289" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Normal 3 3" xfId="290" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="291" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Normal 3 3 2 2 2" xfId="293" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Normal 3 3 2 2 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Normal 3 3 2 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Normal 3 3 2 3" xfId="296" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Normal 3 3 2 3 2" xfId="297" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Normal 3 3 2 4" xfId="298" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="299" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Normal 3 3 3 2" xfId="300" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Normal 3 3 3 2 2" xfId="301" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Normal 3 3 3 3" xfId="302" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Normal 3 3 4" xfId="303" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Normal 3 3 4 2" xfId="304" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Normal 3 3 5" xfId="305" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Normal 3 4" xfId="306" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="307" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Normal 3 4 2 2" xfId="308" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Normal 3 4 2 2 2" xfId="309" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Normal 3 4 2 2 2 2" xfId="310" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Normal 3 4 2 2 3" xfId="311" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Normal 3 4 2 3" xfId="312" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Normal 3 4 2 3 2" xfId="313" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Normal 3 4 2 4" xfId="314" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 3 4 3" xfId="315" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 3 4 3 2" xfId="316" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 3 4 3 2 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 3 4 3 3" xfId="318" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 3 4 4" xfId="319" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 3 4 4 2" xfId="320" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 3 4 5" xfId="321" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 3 5" xfId="322" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 3 5 2" xfId="323" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 3 5 2 2" xfId="324" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 3 5 2 2 2" xfId="325" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 3 5 2 3" xfId="326" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 3 5 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 3 5 3 2" xfId="328" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 3 5 4" xfId="329" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 3 6" xfId="330" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 3 6 2" xfId="331" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 3 6 2 2" xfId="332" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 3 6 3" xfId="333" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 3 7" xfId="334" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 3 7 2" xfId="335" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 3 8" xfId="336" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 4" xfId="337" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="normální_laroux" xfId="338" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 10" xfId="339"/>
-    <cellStyle name="Normalny 10 2" xfId="340"/>
-    <cellStyle name="Normalny 11" xfId="341"/>
-    <cellStyle name="Normalny 11 2" xfId="342"/>
-    <cellStyle name="Normalny 12" xfId="343"/>
-    <cellStyle name="Normalny 12 2" xfId="344"/>
-    <cellStyle name="Normalny 13" xfId="345"/>
-    <cellStyle name="Normalny 13 2" xfId="346"/>
-    <cellStyle name="Normalny 13 2 2" xfId="347"/>
-    <cellStyle name="Normalny 13 2 2 2" xfId="348"/>
-    <cellStyle name="Normalny 13 2 2 2 2" xfId="349"/>
-    <cellStyle name="Normalny 13 2 2 2 2 2" xfId="350"/>
-    <cellStyle name="Normalny 13 2 2 2 3" xfId="351"/>
-    <cellStyle name="Normalny 13 2 2 3" xfId="352"/>
-    <cellStyle name="Normalny 13 2 2 3 2" xfId="353"/>
-    <cellStyle name="Normalny 13 2 2 4" xfId="354"/>
-    <cellStyle name="Normalny 13 2 3" xfId="355"/>
-    <cellStyle name="Normalny 13 2 3 2" xfId="356"/>
-    <cellStyle name="Normalny 13 2 3 2 2" xfId="357"/>
-    <cellStyle name="Normalny 13 2 3 3" xfId="358"/>
-    <cellStyle name="Normalny 13 2 4" xfId="359"/>
-    <cellStyle name="Normalny 13 2 4 2" xfId="360"/>
-    <cellStyle name="Normalny 13 2 5" xfId="361"/>
-    <cellStyle name="Normalny 13 3" xfId="362"/>
-    <cellStyle name="Normalny 13 3 2" xfId="363"/>
-    <cellStyle name="Normalny 13 3 2 2" xfId="364"/>
-    <cellStyle name="Normalny 13 3 2 2 2" xfId="365"/>
-    <cellStyle name="Normalny 13 3 2 2 2 2" xfId="366"/>
-    <cellStyle name="Normalny 13 3 2 2 3" xfId="367"/>
-    <cellStyle name="Normalny 13 3 2 3" xfId="368"/>
-    <cellStyle name="Normalny 13 3 2 3 2" xfId="369"/>
-    <cellStyle name="Normalny 13 3 2 4" xfId="370"/>
-    <cellStyle name="Normalny 13 3 3" xfId="371"/>
-    <cellStyle name="Normalny 13 3 3 2" xfId="372"/>
-    <cellStyle name="Normalny 13 3 3 2 2" xfId="373"/>
-    <cellStyle name="Normalny 13 3 3 3" xfId="374"/>
-    <cellStyle name="Normalny 13 3 4" xfId="375"/>
-    <cellStyle name="Normalny 13 3 4 2" xfId="376"/>
-    <cellStyle name="Normalny 13 3 5" xfId="377"/>
-    <cellStyle name="Normalny 13 4" xfId="378"/>
-    <cellStyle name="Normalny 13 4 2" xfId="379"/>
-    <cellStyle name="Normalny 13 4 2 2" xfId="380"/>
-    <cellStyle name="Normalny 13 4 2 2 2" xfId="381"/>
-    <cellStyle name="Normalny 13 4 2 3" xfId="382"/>
-    <cellStyle name="Normalny 13 4 3" xfId="383"/>
-    <cellStyle name="Normalny 13 4 3 2" xfId="384"/>
-    <cellStyle name="Normalny 13 4 4" xfId="385"/>
-    <cellStyle name="Normalny 13 5" xfId="386"/>
-    <cellStyle name="Normalny 13 5 2" xfId="387"/>
-    <cellStyle name="Normalny 13 5 2 2" xfId="388"/>
-    <cellStyle name="Normalny 13 5 3" xfId="389"/>
-    <cellStyle name="Normalny 13 6" xfId="390"/>
-    <cellStyle name="Normalny 13 6 2" xfId="391"/>
-    <cellStyle name="Normalny 13 7" xfId="392"/>
-    <cellStyle name="Normalny 14" xfId="393"/>
-    <cellStyle name="Normalny 14 2" xfId="394"/>
-    <cellStyle name="Normalny 14 2 2" xfId="395"/>
-    <cellStyle name="Normalny 14 3" xfId="396"/>
-    <cellStyle name="Normalny 15" xfId="397"/>
-    <cellStyle name="Normalny 15 2" xfId="398"/>
-    <cellStyle name="Normalny 16" xfId="399"/>
-    <cellStyle name="Normalny 16 2" xfId="400"/>
-    <cellStyle name="Normalny 17" xfId="401"/>
-    <cellStyle name="Normalny 17 2" xfId="402"/>
-    <cellStyle name="Normalny 18" xfId="403"/>
-    <cellStyle name="Normalny 18 2" xfId="404"/>
-    <cellStyle name="Normalny 19" xfId="405"/>
-    <cellStyle name="Normalny 19 2" xfId="406"/>
-    <cellStyle name="Normalny 2" xfId="1"/>
-    <cellStyle name="Normalny 2 10" xfId="408"/>
-    <cellStyle name="Normalny 2 10 2" xfId="409"/>
-    <cellStyle name="Normalny 2 10 2 2" xfId="410"/>
-    <cellStyle name="Normalny 2 10 2 2 2" xfId="411"/>
-    <cellStyle name="Normalny 2 10 2 3" xfId="412"/>
-    <cellStyle name="Normalny 2 10 3" xfId="413"/>
-    <cellStyle name="Normalny 2 10 3 2" xfId="414"/>
-    <cellStyle name="Normalny 2 10 4" xfId="415"/>
-    <cellStyle name="Normalny 2 11" xfId="416"/>
-    <cellStyle name="Normalny 2 11 2" xfId="417"/>
-    <cellStyle name="Normalny 2 11 2 2" xfId="418"/>
-    <cellStyle name="Normalny 2 11 2 2 2" xfId="419"/>
-    <cellStyle name="Normalny 2 11 2 3" xfId="420"/>
-    <cellStyle name="Normalny 2 11 3" xfId="421"/>
-    <cellStyle name="Normalny 2 11 3 2" xfId="422"/>
-    <cellStyle name="Normalny 2 11 4" xfId="423"/>
-    <cellStyle name="Normalny 2 2" xfId="407"/>
-    <cellStyle name="Normalny 2 2 2" xfId="424"/>
-    <cellStyle name="Normalny 2 3" xfId="425"/>
-    <cellStyle name="Normalny 2 4" xfId="426"/>
-    <cellStyle name="Normalny 2 5" xfId="427"/>
-    <cellStyle name="Normalny 2 6" xfId="428"/>
-    <cellStyle name="Normalny 2 7" xfId="429"/>
-    <cellStyle name="Normalny 2 7 2" xfId="430"/>
-    <cellStyle name="Normalny 2 7 2 2" xfId="431"/>
-    <cellStyle name="Normalny 2 7 2 2 2" xfId="432"/>
-    <cellStyle name="Normalny 2 7 2 2 2 2" xfId="433"/>
-    <cellStyle name="Normalny 2 7 2 2 3" xfId="434"/>
-    <cellStyle name="Normalny 2 7 2 3" xfId="435"/>
-    <cellStyle name="Normalny 2 7 2 3 2" xfId="436"/>
-    <cellStyle name="Normalny 2 7 2 4" xfId="437"/>
-    <cellStyle name="Normalny 2 7 3" xfId="438"/>
-    <cellStyle name="Normalny 2 7 3 2" xfId="439"/>
-    <cellStyle name="Normalny 2 7 3 2 2" xfId="440"/>
-    <cellStyle name="Normalny 2 7 3 3" xfId="441"/>
-    <cellStyle name="Normalny 2 7 4" xfId="442"/>
-    <cellStyle name="Normalny 2 7 4 2" xfId="443"/>
-    <cellStyle name="Normalny 2 7 5" xfId="444"/>
-    <cellStyle name="Normalny 2 8" xfId="445"/>
-    <cellStyle name="Normalny 2 8 2" xfId="446"/>
-    <cellStyle name="Normalny 2 8 2 2" xfId="447"/>
-    <cellStyle name="Normalny 2 8 2 2 2" xfId="448"/>
-    <cellStyle name="Normalny 2 8 2 2 2 2" xfId="449"/>
-    <cellStyle name="Normalny 2 8 2 2 3" xfId="450"/>
-    <cellStyle name="Normalny 2 8 2 3" xfId="451"/>
-    <cellStyle name="Normalny 2 8 2 3 2" xfId="452"/>
-    <cellStyle name="Normalny 2 8 2 4" xfId="453"/>
-    <cellStyle name="Normalny 2 8 3" xfId="454"/>
-    <cellStyle name="Normalny 2 8 3 2" xfId="455"/>
-    <cellStyle name="Normalny 2 8 3 2 2" xfId="456"/>
-    <cellStyle name="Normalny 2 8 3 3" xfId="457"/>
-    <cellStyle name="Normalny 2 8 4" xfId="458"/>
-    <cellStyle name="Normalny 2 8 4 2" xfId="459"/>
-    <cellStyle name="Normalny 2 8 5" xfId="460"/>
-    <cellStyle name="Normalny 2 9" xfId="461"/>
-    <cellStyle name="Normalny 20" xfId="462"/>
-    <cellStyle name="Normalny 20 2" xfId="463"/>
-    <cellStyle name="Normalny 21" xfId="464"/>
-    <cellStyle name="Normalny 21 2" xfId="465"/>
-    <cellStyle name="Normalny 22" xfId="466"/>
-    <cellStyle name="Normalny 22 2" xfId="467"/>
-    <cellStyle name="Normalny 23" xfId="468"/>
-    <cellStyle name="Normalny 23 2" xfId="469"/>
-    <cellStyle name="Normalny 24" xfId="470"/>
-    <cellStyle name="Normalny 24 2" xfId="471"/>
-    <cellStyle name="Normalny 25" xfId="472"/>
-    <cellStyle name="Normalny 25 2" xfId="473"/>
-    <cellStyle name="Normalny 26" xfId="474"/>
-    <cellStyle name="Normalny 26 2" xfId="475"/>
-    <cellStyle name="Normalny 27" xfId="476"/>
-    <cellStyle name="Normalny 27 2" xfId="477"/>
-    <cellStyle name="Normalny 28" xfId="478"/>
-    <cellStyle name="Normalny 28 2" xfId="479"/>
-    <cellStyle name="Normalny 29" xfId="480"/>
-    <cellStyle name="Normalny 29 2" xfId="481"/>
-    <cellStyle name="Normalny 3" xfId="482"/>
-    <cellStyle name="Normalny 3 2" xfId="483"/>
-    <cellStyle name="Normalny 3 2 2" xfId="484"/>
-    <cellStyle name="Normalny 3 2 3" xfId="485"/>
-    <cellStyle name="Normalny 3 2 4" xfId="486"/>
-    <cellStyle name="Normalny 3 3" xfId="487"/>
-    <cellStyle name="Normalny 3 4" xfId="488"/>
-    <cellStyle name="Normalny 3 4 2" xfId="489"/>
-    <cellStyle name="Normalny 3 4 2 2" xfId="490"/>
-    <cellStyle name="Normalny 3 4 3" xfId="491"/>
-    <cellStyle name="Normalny 3 5" xfId="492"/>
-    <cellStyle name="Normalny 3 5 2" xfId="493"/>
-    <cellStyle name="Normalny 3 6" xfId="494"/>
-    <cellStyle name="Normalny 30" xfId="495"/>
-    <cellStyle name="Normalny 30 2" xfId="496"/>
-    <cellStyle name="Normalny 31" xfId="497"/>
-    <cellStyle name="Normalny 31 2" xfId="498"/>
-    <cellStyle name="Normalny 32" xfId="499"/>
-    <cellStyle name="Normalny 32 2" xfId="500"/>
-    <cellStyle name="Normalny 33" xfId="501"/>
-    <cellStyle name="Normalny 33 2" xfId="502"/>
-    <cellStyle name="Normalny 34" xfId="503"/>
-    <cellStyle name="Normalny 34 2" xfId="504"/>
-    <cellStyle name="Normalny 35" xfId="505"/>
-    <cellStyle name="Normalny 35 2" xfId="506"/>
-    <cellStyle name="Normalny 36" xfId="507"/>
-    <cellStyle name="Normalny 36 2" xfId="508"/>
-    <cellStyle name="Normalny 37" xfId="509"/>
-    <cellStyle name="Normalny 37 2" xfId="510"/>
-    <cellStyle name="Normalny 38" xfId="511"/>
-    <cellStyle name="Normalny 38 2" xfId="512"/>
-    <cellStyle name="Normalny 39" xfId="513"/>
-    <cellStyle name="Normalny 39 2" xfId="514"/>
-    <cellStyle name="Normalny 4" xfId="515"/>
-    <cellStyle name="Normalny 4 2" xfId="516"/>
-    <cellStyle name="Normalny 4 3" xfId="517"/>
-    <cellStyle name="Normalny 40" xfId="518"/>
-    <cellStyle name="Normalny 40 2" xfId="519"/>
-    <cellStyle name="Normalny 41" xfId="520"/>
-    <cellStyle name="Normalny 41 2" xfId="521"/>
-    <cellStyle name="Normalny 42" xfId="522"/>
-    <cellStyle name="Normalny 42 2" xfId="523"/>
-    <cellStyle name="Normalny 43" xfId="524"/>
-    <cellStyle name="Normalny 43 2" xfId="525"/>
-    <cellStyle name="Normalny 44" xfId="526"/>
-    <cellStyle name="Normalny 44 2" xfId="527"/>
-    <cellStyle name="Normalny 45" xfId="528"/>
-    <cellStyle name="Normalny 45 2" xfId="529"/>
-    <cellStyle name="Normalny 46" xfId="530"/>
-    <cellStyle name="Normalny 46 2" xfId="531"/>
-    <cellStyle name="Normalny 47" xfId="532"/>
-    <cellStyle name="Normalny 47 2" xfId="533"/>
-    <cellStyle name="Normalny 48" xfId="534"/>
-    <cellStyle name="Normalny 48 2" xfId="535"/>
-    <cellStyle name="Normalny 49" xfId="536"/>
-    <cellStyle name="Normalny 49 2" xfId="537"/>
-    <cellStyle name="Normalny 5" xfId="538"/>
-    <cellStyle name="Normalny 5 2" xfId="539"/>
-    <cellStyle name="Normalny 50" xfId="540"/>
-    <cellStyle name="Normalny 50 2" xfId="541"/>
-    <cellStyle name="Normalny 51" xfId="542"/>
-    <cellStyle name="Normalny 51 2" xfId="543"/>
-    <cellStyle name="Normalny 52" xfId="544"/>
-    <cellStyle name="Normalny 52 2" xfId="545"/>
-    <cellStyle name="Normalny 53" xfId="546"/>
-    <cellStyle name="Normalny 53 2" xfId="547"/>
-    <cellStyle name="Normalny 54" xfId="548"/>
-    <cellStyle name="Normalny 54 2" xfId="549"/>
-    <cellStyle name="Normalny 55" xfId="550"/>
-    <cellStyle name="Normalny 56" xfId="551"/>
-    <cellStyle name="Normalny 56 2" xfId="552"/>
-    <cellStyle name="Normalny 57" xfId="553"/>
-    <cellStyle name="Normalny 57 2" xfId="554"/>
-    <cellStyle name="Normalny 57 3" xfId="555"/>
-    <cellStyle name="Normalny 58" xfId="556"/>
-    <cellStyle name="Normalny 58 2" xfId="557"/>
-    <cellStyle name="Normalny 59" xfId="558"/>
-    <cellStyle name="Normalny 59 2" xfId="559"/>
-    <cellStyle name="Normalny 59 3" xfId="560"/>
-    <cellStyle name="Normalny 6" xfId="561"/>
-    <cellStyle name="Normalny 6 2" xfId="562"/>
-    <cellStyle name="Normalny 60" xfId="563"/>
-    <cellStyle name="Normalny 60 2" xfId="564"/>
-    <cellStyle name="Normalny 61" xfId="565"/>
-    <cellStyle name="Normalny 61 2" xfId="566"/>
-    <cellStyle name="Normalny 61 3" xfId="567"/>
-    <cellStyle name="Normalny 62" xfId="568"/>
-    <cellStyle name="Normalny 62 2" xfId="569"/>
-    <cellStyle name="Normalny 63" xfId="570"/>
-    <cellStyle name="Normalny 63 2" xfId="571"/>
-    <cellStyle name="Normalny 64" xfId="572"/>
-    <cellStyle name="Normalny 64 2" xfId="573"/>
-    <cellStyle name="Normalny 65" xfId="574"/>
-    <cellStyle name="Normalny 66" xfId="575"/>
-    <cellStyle name="Normalny 67" xfId="576"/>
-    <cellStyle name="Normalny 68" xfId="577"/>
-    <cellStyle name="Normalny 68 2" xfId="578"/>
-    <cellStyle name="Normalny 68 2 2" xfId="579"/>
-    <cellStyle name="Normalny 68 3" xfId="580"/>
-    <cellStyle name="Normalny 69" xfId="581"/>
-    <cellStyle name="Normalny 69 2" xfId="582"/>
-    <cellStyle name="Normalny 7" xfId="583"/>
-    <cellStyle name="Normalny 7 2" xfId="584"/>
-    <cellStyle name="Normalny 70" xfId="585"/>
-    <cellStyle name="Normalny 70 2" xfId="586"/>
-    <cellStyle name="Normalny 70 2 2" xfId="587"/>
-    <cellStyle name="Normalny 70 2 2 2" xfId="588"/>
-    <cellStyle name="Normalny 70 2 2 2 2" xfId="589"/>
-    <cellStyle name="Normalny 70 2 2 2 2 2" xfId="590"/>
-    <cellStyle name="Normalny 70 2 2 2 3" xfId="591"/>
-    <cellStyle name="Normalny 70 2 2 3" xfId="592"/>
-    <cellStyle name="Normalny 70 2 2 3 2" xfId="593"/>
-    <cellStyle name="Normalny 70 2 2 4" xfId="594"/>
-    <cellStyle name="Normalny 70 2 3" xfId="595"/>
-    <cellStyle name="Normalny 70 2 3 2" xfId="596"/>
-    <cellStyle name="Normalny 70 2 3 2 2" xfId="597"/>
-    <cellStyle name="Normalny 70 2 3 3" xfId="598"/>
-    <cellStyle name="Normalny 70 2 4" xfId="599"/>
-    <cellStyle name="Normalny 70 2 4 2" xfId="600"/>
-    <cellStyle name="Normalny 70 2 5" xfId="601"/>
-    <cellStyle name="Normalny 70 3" xfId="602"/>
-    <cellStyle name="Normalny 70 3 2" xfId="603"/>
-    <cellStyle name="Normalny 70 3 2 2" xfId="604"/>
-    <cellStyle name="Normalny 70 3 2 2 2" xfId="605"/>
-    <cellStyle name="Normalny 70 3 2 2 2 2" xfId="606"/>
-    <cellStyle name="Normalny 70 3 2 2 3" xfId="607"/>
-    <cellStyle name="Normalny 70 3 2 3" xfId="608"/>
-    <cellStyle name="Normalny 70 3 2 3 2" xfId="609"/>
-    <cellStyle name="Normalny 70 3 2 4" xfId="610"/>
-    <cellStyle name="Normalny 70 3 3" xfId="611"/>
-    <cellStyle name="Normalny 70 3 3 2" xfId="612"/>
-    <cellStyle name="Normalny 70 3 3 2 2" xfId="613"/>
-    <cellStyle name="Normalny 70 3 3 3" xfId="614"/>
-    <cellStyle name="Normalny 70 3 4" xfId="615"/>
-    <cellStyle name="Normalny 70 3 4 2" xfId="616"/>
-    <cellStyle name="Normalny 70 3 5" xfId="617"/>
-    <cellStyle name="Normalny 70 4" xfId="618"/>
-    <cellStyle name="Normalny 70 4 2" xfId="619"/>
-    <cellStyle name="Normalny 70 4 2 2" xfId="620"/>
-    <cellStyle name="Normalny 70 4 2 2 2" xfId="621"/>
-    <cellStyle name="Normalny 70 4 2 3" xfId="622"/>
-    <cellStyle name="Normalny 70 4 3" xfId="623"/>
-    <cellStyle name="Normalny 70 4 3 2" xfId="624"/>
-    <cellStyle name="Normalny 70 4 4" xfId="625"/>
-    <cellStyle name="Normalny 70 5" xfId="626"/>
-    <cellStyle name="Normalny 70 5 2" xfId="627"/>
-    <cellStyle name="Normalny 70 5 2 2" xfId="628"/>
-    <cellStyle name="Normalny 70 5 3" xfId="629"/>
-    <cellStyle name="Normalny 70 6" xfId="630"/>
-    <cellStyle name="Normalny 70 6 2" xfId="631"/>
-    <cellStyle name="Normalny 70 7" xfId="632"/>
-    <cellStyle name="Normalny 71" xfId="633"/>
-    <cellStyle name="Normalny 71 2" xfId="634"/>
-    <cellStyle name="Normalny 71 2 2" xfId="635"/>
-    <cellStyle name="Normalny 71 2 2 2" xfId="636"/>
-    <cellStyle name="Normalny 71 2 2 2 2" xfId="637"/>
-    <cellStyle name="Normalny 71 2 2 2 2 2" xfId="638"/>
-    <cellStyle name="Normalny 71 2 2 2 3" xfId="639"/>
-    <cellStyle name="Normalny 71 2 2 3" xfId="640"/>
-    <cellStyle name="Normalny 71 2 2 3 2" xfId="641"/>
-    <cellStyle name="Normalny 71 2 2 4" xfId="642"/>
-    <cellStyle name="Normalny 71 2 3" xfId="643"/>
-    <cellStyle name="Normalny 71 2 3 2" xfId="644"/>
-    <cellStyle name="Normalny 71 2 3 2 2" xfId="645"/>
-    <cellStyle name="Normalny 71 2 3 3" xfId="646"/>
-    <cellStyle name="Normalny 71 2 4" xfId="647"/>
-    <cellStyle name="Normalny 71 2 4 2" xfId="648"/>
-    <cellStyle name="Normalny 71 2 5" xfId="649"/>
-    <cellStyle name="Normalny 71 3" xfId="650"/>
-    <cellStyle name="Normalny 71 3 2" xfId="651"/>
-    <cellStyle name="Normalny 71 3 2 2" xfId="652"/>
-    <cellStyle name="Normalny 71 3 2 2 2" xfId="653"/>
-    <cellStyle name="Normalny 71 3 2 3" xfId="654"/>
-    <cellStyle name="Normalny 71 3 3" xfId="655"/>
-    <cellStyle name="Normalny 71 3 3 2" xfId="656"/>
-    <cellStyle name="Normalny 71 3 4" xfId="657"/>
-    <cellStyle name="Normalny 71 4" xfId="658"/>
-    <cellStyle name="Normalny 71 4 2" xfId="659"/>
-    <cellStyle name="Normalny 71 4 2 2" xfId="660"/>
-    <cellStyle name="Normalny 71 4 3" xfId="661"/>
-    <cellStyle name="Normalny 71 5" xfId="662"/>
-    <cellStyle name="Normalny 71 5 2" xfId="663"/>
-    <cellStyle name="Normalny 71 6" xfId="664"/>
-    <cellStyle name="Normalny 72" xfId="665"/>
-    <cellStyle name="Normalny 72 2" xfId="666"/>
-    <cellStyle name="Normalny 72 2 2" xfId="667"/>
-    <cellStyle name="Normalny 72 2 2 2" xfId="668"/>
-    <cellStyle name="Normalny 72 2 2 2 2" xfId="669"/>
-    <cellStyle name="Normalny 72 2 2 2 2 2" xfId="670"/>
-    <cellStyle name="Normalny 72 2 2 2 3" xfId="671"/>
-    <cellStyle name="Normalny 72 2 2 3" xfId="672"/>
-    <cellStyle name="Normalny 72 2 2 3 2" xfId="673"/>
-    <cellStyle name="Normalny 72 2 2 4" xfId="674"/>
-    <cellStyle name="Normalny 72 2 3" xfId="675"/>
-    <cellStyle name="Normalny 72 2 3 2" xfId="676"/>
-    <cellStyle name="Normalny 72 2 3 2 2" xfId="677"/>
-    <cellStyle name="Normalny 72 2 3 3" xfId="678"/>
-    <cellStyle name="Normalny 72 2 4" xfId="679"/>
-    <cellStyle name="Normalny 72 2 4 2" xfId="680"/>
-    <cellStyle name="Normalny 72 2 5" xfId="681"/>
-    <cellStyle name="Normalny 72 3" xfId="682"/>
-    <cellStyle name="Normalny 72 3 2" xfId="683"/>
-    <cellStyle name="Normalny 72 3 2 2" xfId="684"/>
-    <cellStyle name="Normalny 72 3 2 2 2" xfId="685"/>
-    <cellStyle name="Normalny 72 3 2 3" xfId="686"/>
-    <cellStyle name="Normalny 72 3 3" xfId="687"/>
-    <cellStyle name="Normalny 72 3 3 2" xfId="688"/>
-    <cellStyle name="Normalny 72 3 4" xfId="689"/>
-    <cellStyle name="Normalny 72 4" xfId="690"/>
-    <cellStyle name="Normalny 72 4 2" xfId="691"/>
-    <cellStyle name="Normalny 72 4 2 2" xfId="692"/>
-    <cellStyle name="Normalny 72 4 3" xfId="693"/>
-    <cellStyle name="Normalny 72 5" xfId="694"/>
-    <cellStyle name="Normalny 72 5 2" xfId="695"/>
-    <cellStyle name="Normalny 72 6" xfId="696"/>
-    <cellStyle name="Normalny 73" xfId="697"/>
-    <cellStyle name="Normalny 73 2" xfId="698"/>
-    <cellStyle name="Normalny 73 2 2" xfId="699"/>
-    <cellStyle name="Normalny 73 2 2 2" xfId="700"/>
-    <cellStyle name="Normalny 73 2 2 2 2" xfId="701"/>
-    <cellStyle name="Normalny 73 2 2 2 2 2" xfId="702"/>
-    <cellStyle name="Normalny 73 2 2 2 3" xfId="703"/>
-    <cellStyle name="Normalny 73 2 2 3" xfId="704"/>
-    <cellStyle name="Normalny 73 2 2 3 2" xfId="705"/>
-    <cellStyle name="Normalny 73 2 2 4" xfId="706"/>
-    <cellStyle name="Normalny 73 2 3" xfId="707"/>
-    <cellStyle name="Normalny 73 2 3 2" xfId="708"/>
-    <cellStyle name="Normalny 73 2 3 2 2" xfId="709"/>
-    <cellStyle name="Normalny 73 2 3 3" xfId="710"/>
-    <cellStyle name="Normalny 73 2 4" xfId="711"/>
-    <cellStyle name="Normalny 73 2 4 2" xfId="712"/>
-    <cellStyle name="Normalny 73 2 5" xfId="713"/>
-    <cellStyle name="Normalny 73 3" xfId="714"/>
-    <cellStyle name="Normalny 73 3 2" xfId="715"/>
-    <cellStyle name="Normalny 73 3 2 2" xfId="716"/>
-    <cellStyle name="Normalny 73 3 2 2 2" xfId="717"/>
-    <cellStyle name="Normalny 73 3 2 3" xfId="718"/>
-    <cellStyle name="Normalny 73 3 3" xfId="719"/>
-    <cellStyle name="Normalny 73 3 3 2" xfId="720"/>
-    <cellStyle name="Normalny 73 3 4" xfId="721"/>
-    <cellStyle name="Normalny 73 4" xfId="722"/>
-    <cellStyle name="Normalny 73 4 2" xfId="723"/>
-    <cellStyle name="Normalny 73 4 2 2" xfId="724"/>
-    <cellStyle name="Normalny 73 4 3" xfId="725"/>
-    <cellStyle name="Normalny 73 5" xfId="726"/>
-    <cellStyle name="Normalny 73 5 2" xfId="727"/>
-    <cellStyle name="Normalny 73 6" xfId="728"/>
-    <cellStyle name="Normalny 74" xfId="729"/>
-    <cellStyle name="Normalny 74 2" xfId="730"/>
-    <cellStyle name="Normalny 74 2 2" xfId="731"/>
-    <cellStyle name="Normalny 74 2 2 2" xfId="732"/>
-    <cellStyle name="Normalny 74 2 2 2 2" xfId="733"/>
-    <cellStyle name="Normalny 74 2 2 2 2 2" xfId="734"/>
-    <cellStyle name="Normalny 74 2 2 2 3" xfId="735"/>
-    <cellStyle name="Normalny 74 2 2 3" xfId="736"/>
-    <cellStyle name="Normalny 74 2 2 3 2" xfId="737"/>
-    <cellStyle name="Normalny 74 2 2 4" xfId="738"/>
-    <cellStyle name="Normalny 74 2 3" xfId="739"/>
-    <cellStyle name="Normalny 74 2 3 2" xfId="740"/>
-    <cellStyle name="Normalny 74 2 3 2 2" xfId="741"/>
-    <cellStyle name="Normalny 74 2 3 3" xfId="742"/>
-    <cellStyle name="Normalny 74 2 4" xfId="743"/>
-    <cellStyle name="Normalny 74 2 4 2" xfId="744"/>
-    <cellStyle name="Normalny 74 2 5" xfId="745"/>
-    <cellStyle name="Normalny 74 3" xfId="746"/>
-    <cellStyle name="Normalny 74 3 2" xfId="747"/>
-    <cellStyle name="Normalny 74 3 2 2" xfId="748"/>
-    <cellStyle name="Normalny 74 3 2 2 2" xfId="749"/>
-    <cellStyle name="Normalny 74 3 2 3" xfId="750"/>
-    <cellStyle name="Normalny 74 3 3" xfId="751"/>
-    <cellStyle name="Normalny 74 3 3 2" xfId="752"/>
-    <cellStyle name="Normalny 74 3 4" xfId="753"/>
-    <cellStyle name="Normalny 74 4" xfId="754"/>
-    <cellStyle name="Normalny 74 4 2" xfId="755"/>
-    <cellStyle name="Normalny 74 4 2 2" xfId="756"/>
-    <cellStyle name="Normalny 74 4 3" xfId="757"/>
-    <cellStyle name="Normalny 74 5" xfId="758"/>
-    <cellStyle name="Normalny 74 5 2" xfId="759"/>
-    <cellStyle name="Normalny 74 6" xfId="760"/>
-    <cellStyle name="Normalny 75" xfId="761"/>
-    <cellStyle name="Normalny 75 2" xfId="762"/>
-    <cellStyle name="Normalny 75 2 2" xfId="763"/>
-    <cellStyle name="Normalny 75 2 2 2" xfId="764"/>
-    <cellStyle name="Normalny 75 2 3" xfId="765"/>
-    <cellStyle name="Normalny 75 3" xfId="766"/>
-    <cellStyle name="Normalny 75 3 2" xfId="767"/>
-    <cellStyle name="Normalny 75 4" xfId="768"/>
-    <cellStyle name="Normalny 76" xfId="769"/>
-    <cellStyle name="Normalny 77" xfId="770"/>
-    <cellStyle name="Normalny 77 2" xfId="771"/>
-    <cellStyle name="Normalny 77 2 2" xfId="772"/>
-    <cellStyle name="Normalny 77 3" xfId="773"/>
-    <cellStyle name="Normalny 78" xfId="774"/>
-    <cellStyle name="Normalny 79" xfId="775"/>
-    <cellStyle name="Normalny 79 2" xfId="776"/>
-    <cellStyle name="Normalny 8" xfId="777"/>
-    <cellStyle name="Normalny 8 2" xfId="778"/>
-    <cellStyle name="Normalny 80" xfId="779"/>
-    <cellStyle name="Normalny 81" xfId="780"/>
-    <cellStyle name="Normalny 9" xfId="781"/>
-    <cellStyle name="Normalny 9 2" xfId="782"/>
-    <cellStyle name="Opis" xfId="783"/>
-    <cellStyle name="Percent [2]" xfId="784"/>
-    <cellStyle name="Percent [2] 2" xfId="785"/>
-    <cellStyle name="Percent 2" xfId="786"/>
-    <cellStyle name="Percent 2 2" xfId="787"/>
-    <cellStyle name="Percent 2 2 2" xfId="788"/>
-    <cellStyle name="Percent 2 3" xfId="789"/>
-    <cellStyle name="Percent 2 3 2" xfId="790"/>
-    <cellStyle name="Percent 2 3 2 2" xfId="791"/>
-    <cellStyle name="Percent 2 3 2 2 2" xfId="792"/>
-    <cellStyle name="Percent 2 3 2 2 2 2" xfId="793"/>
-    <cellStyle name="Percent 2 3 2 2 3" xfId="794"/>
-    <cellStyle name="Percent 2 3 2 3" xfId="795"/>
-    <cellStyle name="Percent 2 3 2 3 2" xfId="796"/>
-    <cellStyle name="Percent 2 3 2 4" xfId="797"/>
-    <cellStyle name="Percent 2 3 3" xfId="798"/>
-    <cellStyle name="Percent 2 3 3 2" xfId="799"/>
-    <cellStyle name="Percent 2 3 3 2 2" xfId="800"/>
-    <cellStyle name="Percent 2 3 3 3" xfId="801"/>
-    <cellStyle name="Percent 2 3 4" xfId="802"/>
-    <cellStyle name="Percent 2 3 4 2" xfId="803"/>
-    <cellStyle name="Percent 2 3 5" xfId="804"/>
-    <cellStyle name="Percent 2 4" xfId="805"/>
-    <cellStyle name="Percent 2 4 2" xfId="806"/>
-    <cellStyle name="Percent 2 4 2 2" xfId="807"/>
-    <cellStyle name="Percent 2 4 2 2 2" xfId="808"/>
-    <cellStyle name="Percent 2 4 2 2 2 2" xfId="809"/>
-    <cellStyle name="Percent 2 4 2 2 3" xfId="810"/>
-    <cellStyle name="Percent 2 4 2 3" xfId="811"/>
-    <cellStyle name="Percent 2 4 2 3 2" xfId="812"/>
-    <cellStyle name="Percent 2 4 2 4" xfId="813"/>
-    <cellStyle name="Percent 2 4 3" xfId="814"/>
-    <cellStyle name="Percent 2 4 3 2" xfId="815"/>
-    <cellStyle name="Percent 2 4 3 2 2" xfId="816"/>
-    <cellStyle name="Percent 2 4 3 3" xfId="817"/>
-    <cellStyle name="Percent 2 4 4" xfId="818"/>
-    <cellStyle name="Percent 2 4 4 2" xfId="819"/>
-    <cellStyle name="Percent 2 4 5" xfId="820"/>
-    <cellStyle name="Percent 2 5" xfId="821"/>
-    <cellStyle name="Percent 2 5 2" xfId="822"/>
-    <cellStyle name="Percent 2 5 2 2" xfId="823"/>
-    <cellStyle name="Percent 2 5 2 2 2" xfId="824"/>
-    <cellStyle name="Percent 2 5 2 3" xfId="825"/>
-    <cellStyle name="Percent 2 5 3" xfId="826"/>
-    <cellStyle name="Percent 2 5 3 2" xfId="827"/>
-    <cellStyle name="Percent 2 5 4" xfId="828"/>
-    <cellStyle name="Percent 2 6" xfId="829"/>
-    <cellStyle name="Percent 2 6 2" xfId="830"/>
-    <cellStyle name="Percent 2 6 2 2" xfId="831"/>
-    <cellStyle name="Percent 2 6 3" xfId="832"/>
-    <cellStyle name="Percent 2 7" xfId="833"/>
-    <cellStyle name="Percent 2 7 2" xfId="834"/>
-    <cellStyle name="Percent 2 8" xfId="835"/>
-    <cellStyle name="Percent 3" xfId="836"/>
-    <cellStyle name="Percent 3 2" xfId="837"/>
-    <cellStyle name="Percent 3 2 2" xfId="838"/>
-    <cellStyle name="Percent 3 2 2 2" xfId="839"/>
-    <cellStyle name="Percent 3 2 2 2 2" xfId="840"/>
-    <cellStyle name="Percent 3 2 2 2 2 2" xfId="841"/>
-    <cellStyle name="Percent 3 2 2 2 3" xfId="842"/>
-    <cellStyle name="Percent 3 2 2 3" xfId="843"/>
-    <cellStyle name="Percent 3 2 2 3 2" xfId="844"/>
-    <cellStyle name="Percent 3 2 2 4" xfId="845"/>
-    <cellStyle name="Percent 3 2 3" xfId="846"/>
-    <cellStyle name="Percent 3 2 3 2" xfId="847"/>
-    <cellStyle name="Percent 3 2 3 2 2" xfId="848"/>
-    <cellStyle name="Percent 3 2 3 3" xfId="849"/>
-    <cellStyle name="Percent 3 2 4" xfId="850"/>
-    <cellStyle name="Percent 3 2 4 2" xfId="851"/>
-    <cellStyle name="Percent 3 2 5" xfId="852"/>
-    <cellStyle name="Percent 3 3" xfId="853"/>
-    <cellStyle name="Percent 3 3 2" xfId="854"/>
-    <cellStyle name="Percent 3 3 2 2" xfId="855"/>
-    <cellStyle name="Percent 3 3 2 2 2" xfId="856"/>
-    <cellStyle name="Percent 3 3 2 2 2 2" xfId="857"/>
-    <cellStyle name="Percent 3 3 2 2 3" xfId="858"/>
-    <cellStyle name="Percent 3 3 2 3" xfId="859"/>
-    <cellStyle name="Percent 3 3 2 3 2" xfId="860"/>
-    <cellStyle name="Percent 3 3 2 4" xfId="861"/>
-    <cellStyle name="Percent 3 3 3" xfId="862"/>
-    <cellStyle name="Percent 3 3 3 2" xfId="863"/>
-    <cellStyle name="Percent 3 3 3 2 2" xfId="864"/>
-    <cellStyle name="Percent 3 3 3 3" xfId="865"/>
-    <cellStyle name="Percent 3 3 4" xfId="866"/>
-    <cellStyle name="Percent 3 3 4 2" xfId="867"/>
-    <cellStyle name="Percent 3 3 5" xfId="868"/>
-    <cellStyle name="Percent 3 4" xfId="869"/>
-    <cellStyle name="Percent 3 4 2" xfId="870"/>
-    <cellStyle name="Percent 3 4 2 2" xfId="871"/>
-    <cellStyle name="Percent 3 4 2 2 2" xfId="872"/>
-    <cellStyle name="Percent 3 4 2 3" xfId="873"/>
-    <cellStyle name="Percent 3 4 3" xfId="874"/>
-    <cellStyle name="Percent 3 4 3 2" xfId="875"/>
-    <cellStyle name="Percent 3 4 4" xfId="876"/>
-    <cellStyle name="Percent 3 5" xfId="877"/>
-    <cellStyle name="Percent 3 5 2" xfId="878"/>
-    <cellStyle name="Percent 3 5 2 2" xfId="879"/>
-    <cellStyle name="Percent 3 5 3" xfId="880"/>
-    <cellStyle name="Percent 3 6" xfId="881"/>
-    <cellStyle name="Percent 3 6 2" xfId="882"/>
-    <cellStyle name="Percent 3 7" xfId="883"/>
-    <cellStyle name="Procentowy 2" xfId="884"/>
-    <cellStyle name="Procentowy 2 2" xfId="885"/>
-    <cellStyle name="Procentowy 2 2 2" xfId="886"/>
-    <cellStyle name="Procentowy 2 3" xfId="887"/>
-    <cellStyle name="Procentowy 2 3 2" xfId="888"/>
-    <cellStyle name="Procentowy 2 3 2 2" xfId="889"/>
-    <cellStyle name="Procentowy 2 4" xfId="890"/>
-    <cellStyle name="Procentowy 2 5" xfId="891"/>
-    <cellStyle name="Procentowy 3" xfId="892"/>
-    <cellStyle name="Procentowy 3 2" xfId="893"/>
-    <cellStyle name="Procentowy 3 2 2" xfId="894"/>
-    <cellStyle name="Procentowy 3 2 2 2" xfId="895"/>
-    <cellStyle name="Procentowy 3 2 2 2 2" xfId="896"/>
-    <cellStyle name="Procentowy 3 2 2 2 2 2" xfId="897"/>
-    <cellStyle name="Procentowy 3 2 2 2 3" xfId="898"/>
-    <cellStyle name="Procentowy 3 2 2 3" xfId="899"/>
-    <cellStyle name="Procentowy 3 2 2 3 2" xfId="900"/>
-    <cellStyle name="Procentowy 3 2 2 4" xfId="901"/>
-    <cellStyle name="Procentowy 3 2 3" xfId="902"/>
-    <cellStyle name="Procentowy 3 2 3 2" xfId="903"/>
-    <cellStyle name="Procentowy 3 2 3 2 2" xfId="904"/>
-    <cellStyle name="Procentowy 3 2 3 3" xfId="905"/>
-    <cellStyle name="Procentowy 3 2 4" xfId="906"/>
-    <cellStyle name="Procentowy 3 2 4 2" xfId="907"/>
-    <cellStyle name="Procentowy 3 2 5" xfId="908"/>
-    <cellStyle name="Procentowy 3 3" xfId="909"/>
-    <cellStyle name="Procentowy 3 3 2" xfId="910"/>
-    <cellStyle name="Procentowy 3 3 2 2" xfId="911"/>
-    <cellStyle name="Procentowy 3 3 2 2 2" xfId="912"/>
-    <cellStyle name="Procentowy 3 3 2 2 2 2" xfId="913"/>
-    <cellStyle name="Procentowy 3 3 2 2 3" xfId="914"/>
-    <cellStyle name="Procentowy 3 3 2 3" xfId="915"/>
-    <cellStyle name="Procentowy 3 3 2 3 2" xfId="916"/>
-    <cellStyle name="Procentowy 3 3 2 4" xfId="917"/>
-    <cellStyle name="Procentowy 3 3 3" xfId="918"/>
-    <cellStyle name="Procentowy 3 3 3 2" xfId="919"/>
-    <cellStyle name="Procentowy 3 3 3 2 2" xfId="920"/>
-    <cellStyle name="Procentowy 3 3 3 3" xfId="921"/>
-    <cellStyle name="Procentowy 3 3 4" xfId="922"/>
-    <cellStyle name="Procentowy 3 3 4 2" xfId="923"/>
-    <cellStyle name="Procentowy 3 3 5" xfId="924"/>
-    <cellStyle name="Procentowy 3 4" xfId="925"/>
-    <cellStyle name="Procentowy 3 4 2" xfId="926"/>
-    <cellStyle name="Procentowy 3 4 2 2" xfId="927"/>
-    <cellStyle name="Procentowy 3 4 2 2 2" xfId="928"/>
-    <cellStyle name="Procentowy 3 4 2 3" xfId="929"/>
-    <cellStyle name="Procentowy 3 4 3" xfId="930"/>
-    <cellStyle name="Procentowy 3 4 3 2" xfId="931"/>
-    <cellStyle name="Procentowy 3 4 4" xfId="932"/>
-    <cellStyle name="Procentowy 3 5" xfId="933"/>
-    <cellStyle name="Procentowy 3 5 2" xfId="934"/>
-    <cellStyle name="Procentowy 3 5 2 2" xfId="935"/>
-    <cellStyle name="Procentowy 3 5 3" xfId="936"/>
-    <cellStyle name="Procentowy 3 6" xfId="937"/>
-    <cellStyle name="Procentowy 3 6 2" xfId="938"/>
-    <cellStyle name="Procentowy 3 7" xfId="939"/>
-    <cellStyle name="Procentowy 4" xfId="940"/>
-    <cellStyle name="Procentowy 4 2" xfId="941"/>
-    <cellStyle name="Procentowy 4 3" xfId="942"/>
-    <cellStyle name="Procentowy 4 3 2" xfId="943"/>
-    <cellStyle name="Procentowy 4 3 2 2" xfId="944"/>
-    <cellStyle name="Procentowy 4 3 3" xfId="945"/>
-    <cellStyle name="Procentowy 4 4" xfId="946"/>
-    <cellStyle name="Procentowy 4 4 2" xfId="947"/>
-    <cellStyle name="Procentowy 4 5" xfId="948"/>
-    <cellStyle name="Procentowy 5" xfId="949"/>
-    <cellStyle name="Styl 1" xfId="950"/>
-    <cellStyle name="Uwaga 2" xfId="951"/>
-    <cellStyle name="Uwaga 2 2" xfId="952"/>
-    <cellStyle name="Uwaga 3" xfId="953"/>
-    <cellStyle name="Uwaga 3 2" xfId="954"/>
-    <cellStyle name="Walutowy 2" xfId="955"/>
-    <cellStyle name="Walutowy 2 2" xfId="956"/>
-    <cellStyle name="Walutowy 2 2 2" xfId="957"/>
-    <cellStyle name="Walutowy 2 3" xfId="958"/>
-    <cellStyle name="Walutowy 2 3 2" xfId="959"/>
-    <cellStyle name="Walutowy 2 3 2 2" xfId="960"/>
-    <cellStyle name="Walutowy 2 4" xfId="961"/>
-    <cellStyle name="Walutowy 2 5" xfId="962"/>
-    <cellStyle name="Walutowy 3" xfId="963"/>
-    <cellStyle name="Walutowy 3 2" xfId="964"/>
-    <cellStyle name="Walutowy 3 2 2" xfId="965"/>
-    <cellStyle name="Walutowy 3 2 2 2" xfId="966"/>
-    <cellStyle name="Walutowy 3 2 2 2 2" xfId="967"/>
-    <cellStyle name="Walutowy 3 2 2 2 2 2" xfId="968"/>
-    <cellStyle name="Walutowy 3 2 2 2 3" xfId="969"/>
-    <cellStyle name="Walutowy 3 2 2 3" xfId="970"/>
-    <cellStyle name="Walutowy 3 2 2 3 2" xfId="971"/>
-    <cellStyle name="Walutowy 3 2 2 4" xfId="972"/>
-    <cellStyle name="Walutowy 3 2 3" xfId="973"/>
-    <cellStyle name="Walutowy 3 2 3 2" xfId="974"/>
-    <cellStyle name="Walutowy 3 2 3 2 2" xfId="975"/>
-    <cellStyle name="Walutowy 3 2 3 3" xfId="976"/>
-    <cellStyle name="Walutowy 3 2 4" xfId="977"/>
-    <cellStyle name="Walutowy 3 2 4 2" xfId="978"/>
-    <cellStyle name="Walutowy 3 2 5" xfId="979"/>
-    <cellStyle name="Walutowy 3 3" xfId="980"/>
-    <cellStyle name="Walutowy 3 3 2" xfId="981"/>
-    <cellStyle name="Walutowy 3 3 2 2" xfId="982"/>
-    <cellStyle name="Walutowy 3 3 2 2 2" xfId="983"/>
-    <cellStyle name="Walutowy 3 3 2 2 2 2" xfId="984"/>
-    <cellStyle name="Walutowy 3 3 2 2 3" xfId="985"/>
-    <cellStyle name="Walutowy 3 3 2 3" xfId="986"/>
-    <cellStyle name="Walutowy 3 3 2 3 2" xfId="987"/>
-    <cellStyle name="Walutowy 3 3 2 4" xfId="988"/>
-    <cellStyle name="Walutowy 3 4" xfId="989"/>
-    <cellStyle name="Walutowy 3 4 2" xfId="990"/>
-    <cellStyle name="Walutowy 3 4 2 2" xfId="991"/>
-    <cellStyle name="Walutowy 3 4 3" xfId="992"/>
-    <cellStyle name="Walutowy 3 5" xfId="993"/>
-    <cellStyle name="Walutowy 3 5 2" xfId="994"/>
-    <cellStyle name="Walutowy 3 6" xfId="995"/>
-    <cellStyle name="Walutowy 4" xfId="996"/>
-    <cellStyle name="Walutowy 4 2" xfId="997"/>
-    <cellStyle name="Walutowy 4 2 2" xfId="998"/>
-    <cellStyle name="Walutowy 4 2 2 2" xfId="999"/>
-    <cellStyle name="Walutowy 4 2 2 2 2" xfId="1000"/>
-    <cellStyle name="Walutowy 4 2 2 2 2 2" xfId="1001"/>
-    <cellStyle name="Walutowy 4 2 2 2 3" xfId="1002"/>
-    <cellStyle name="Walutowy 4 2 2 3" xfId="1003"/>
-    <cellStyle name="Walutowy 4 2 2 3 2" xfId="1004"/>
-    <cellStyle name="Walutowy 4 2 2 4" xfId="1005"/>
-    <cellStyle name="Walutowy 4 2 3" xfId="1006"/>
-    <cellStyle name="Walutowy 4 2 3 2" xfId="1007"/>
-    <cellStyle name="Walutowy 4 2 3 2 2" xfId="1008"/>
-    <cellStyle name="Walutowy 4 2 3 3" xfId="1009"/>
-    <cellStyle name="Walutowy 4 2 4" xfId="1010"/>
-    <cellStyle name="Walutowy 4 2 4 2" xfId="1011"/>
-    <cellStyle name="Walutowy 4 2 5" xfId="1012"/>
-    <cellStyle name="Walutowy 4 3" xfId="1013"/>
-    <cellStyle name="Walutowy 4 3 2" xfId="1014"/>
-    <cellStyle name="Walutowy 4 3 2 2" xfId="1015"/>
-    <cellStyle name="Walutowy 4 3 2 2 2" xfId="1016"/>
-    <cellStyle name="Walutowy 4 3 2 3" xfId="1017"/>
-    <cellStyle name="Walutowy 4 3 3" xfId="1018"/>
-    <cellStyle name="Walutowy 4 3 3 2" xfId="1019"/>
-    <cellStyle name="Walutowy 4 3 4" xfId="1020"/>
-    <cellStyle name="Walutowy 4 4" xfId="1021"/>
-    <cellStyle name="Walutowy 4 4 2" xfId="1022"/>
-    <cellStyle name="Walutowy 4 4 2 2" xfId="1023"/>
-    <cellStyle name="Walutowy 4 4 3" xfId="1024"/>
-    <cellStyle name="Walutowy 4 5" xfId="1025"/>
-    <cellStyle name="Walutowy 4 5 2" xfId="1026"/>
-    <cellStyle name="Walutowy 4 6" xfId="1027"/>
-    <cellStyle name="Walutowy 5" xfId="1028"/>
-    <cellStyle name="Walutowy 5 2" xfId="1029"/>
-    <cellStyle name="Walutowy 5 2 2" xfId="1030"/>
-    <cellStyle name="Walutowy 5 2 2 2" xfId="1031"/>
-    <cellStyle name="Walutowy 5 2 2 2 2" xfId="1032"/>
-    <cellStyle name="Walutowy 5 2 2 2 2 2" xfId="1033"/>
-    <cellStyle name="Walutowy 5 2 2 2 3" xfId="1034"/>
-    <cellStyle name="Walutowy 5 2 2 3" xfId="1035"/>
-    <cellStyle name="Walutowy 5 2 2 3 2" xfId="1036"/>
-    <cellStyle name="Walutowy 5 2 2 4" xfId="1037"/>
-    <cellStyle name="Walutowy 5 2 3" xfId="1038"/>
-    <cellStyle name="Walutowy 5 2 3 2" xfId="1039"/>
-    <cellStyle name="Walutowy 5 2 3 2 2" xfId="1040"/>
-    <cellStyle name="Walutowy 5 2 3 3" xfId="1041"/>
-    <cellStyle name="Walutowy 5 2 4" xfId="1042"/>
-    <cellStyle name="Walutowy 5 2 4 2" xfId="1043"/>
-    <cellStyle name="Walutowy 5 2 5" xfId="1044"/>
-    <cellStyle name="Walutowy 5 3" xfId="1045"/>
-    <cellStyle name="Walutowy 5 3 2" xfId="1046"/>
-    <cellStyle name="Walutowy 5 3 2 2" xfId="1047"/>
-    <cellStyle name="Walutowy 5 3 2 2 2" xfId="1048"/>
-    <cellStyle name="Walutowy 5 3 2 3" xfId="1049"/>
-    <cellStyle name="Walutowy 5 3 3" xfId="1050"/>
-    <cellStyle name="Walutowy 5 3 3 2" xfId="1051"/>
-    <cellStyle name="Walutowy 5 3 4" xfId="1052"/>
-    <cellStyle name="Walutowy 5 4" xfId="1053"/>
-    <cellStyle name="Walutowy 5 4 2" xfId="1054"/>
-    <cellStyle name="Walutowy 5 4 2 2" xfId="1055"/>
-    <cellStyle name="Walutowy 5 4 3" xfId="1056"/>
-    <cellStyle name="Walutowy 5 5" xfId="1057"/>
-    <cellStyle name="Walutowy 5 5 2" xfId="1058"/>
-    <cellStyle name="Walutowy 5 6" xfId="1059"/>
-    <cellStyle name="Walutowy 6" xfId="1060"/>
-    <cellStyle name="Walutowy 6 2" xfId="1061"/>
-    <cellStyle name="Walutowy 6 2 2" xfId="1062"/>
-    <cellStyle name="Walutowy 6 2 2 2" xfId="1063"/>
-    <cellStyle name="Walutowy 6 2 2 2 2" xfId="1064"/>
-    <cellStyle name="Walutowy 6 2 2 2 2 2" xfId="1065"/>
-    <cellStyle name="Walutowy 6 2 2 2 3" xfId="1066"/>
-    <cellStyle name="Walutowy 6 2 2 3" xfId="1067"/>
-    <cellStyle name="Walutowy 6 2 2 3 2" xfId="1068"/>
-    <cellStyle name="Walutowy 6 2 2 4" xfId="1069"/>
-    <cellStyle name="Walutowy 6 2 3" xfId="1070"/>
-    <cellStyle name="Walutowy 6 2 3 2" xfId="1071"/>
-    <cellStyle name="Walutowy 6 2 3 2 2" xfId="1072"/>
-    <cellStyle name="Walutowy 6 2 3 3" xfId="1073"/>
-    <cellStyle name="Walutowy 6 2 4" xfId="1074"/>
-    <cellStyle name="Walutowy 6 2 4 2" xfId="1075"/>
-    <cellStyle name="Walutowy 6 2 5" xfId="1076"/>
-    <cellStyle name="Walutowy 6 3" xfId="1077"/>
-    <cellStyle name="Walutowy 6 3 2" xfId="1078"/>
-    <cellStyle name="Walutowy 6 3 2 2" xfId="1079"/>
-    <cellStyle name="Walutowy 6 3 2 2 2" xfId="1080"/>
-    <cellStyle name="Walutowy 6 3 2 3" xfId="1081"/>
-    <cellStyle name="Walutowy 6 3 3" xfId="1082"/>
-    <cellStyle name="Walutowy 6 3 3 2" xfId="1083"/>
-    <cellStyle name="Walutowy 6 3 4" xfId="1084"/>
-    <cellStyle name="Walutowy 6 4" xfId="1085"/>
-    <cellStyle name="Walutowy 6 4 2" xfId="1086"/>
-    <cellStyle name="Walutowy 6 4 2 2" xfId="1087"/>
-    <cellStyle name="Walutowy 6 4 3" xfId="1088"/>
-    <cellStyle name="Walutowy 6 5" xfId="1089"/>
-    <cellStyle name="Walutowy 6 5 2" xfId="1090"/>
-    <cellStyle name="Walutowy 6 6" xfId="1091"/>
-    <cellStyle name="Walutowy 7" xfId="1092"/>
-    <cellStyle name="Walutowy 7 2" xfId="1093"/>
-    <cellStyle name="Walutowy 7 2 2" xfId="1094"/>
-    <cellStyle name="Walutowy 7 2 2 2" xfId="1095"/>
-    <cellStyle name="Walutowy 7 2 3" xfId="1096"/>
-    <cellStyle name="Walutowy 7 3" xfId="1097"/>
-    <cellStyle name="Walutowy 7 3 2" xfId="1098"/>
-    <cellStyle name="Walutowy 7 4" xfId="1099"/>
-    <cellStyle name="Walutowy 8" xfId="1100"/>
+    <cellStyle name="Normalny 10" xfId="339" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normalny 10 2" xfId="340" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normalny 11" xfId="341" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normalny 11 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normalny 12" xfId="343" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normalny 12 2" xfId="344" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normalny 13" xfId="345" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normalny 13 2" xfId="346" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normalny 13 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normalny 13 2 2 2" xfId="348" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normalny 13 2 2 2 2" xfId="349" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normalny 13 2 2 2 2 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normalny 13 2 2 2 3" xfId="351" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normalny 13 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normalny 13 2 2 3 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normalny 13 2 2 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normalny 13 2 3" xfId="355" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normalny 13 2 3 2" xfId="356" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normalny 13 2 3 2 2" xfId="357" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normalny 13 2 3 3" xfId="358" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normalny 13 2 4" xfId="359" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normalny 13 2 4 2" xfId="360" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normalny 13 2 5" xfId="361" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normalny 13 3" xfId="362" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normalny 13 3 2" xfId="363" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normalny 13 3 2 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normalny 13 3 2 2 2" xfId="365" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normalny 13 3 2 2 2 2" xfId="366" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normalny 13 3 2 2 3" xfId="367" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Normalny 13 3 2 3" xfId="368" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Normalny 13 3 2 3 2" xfId="369" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Normalny 13 3 2 4" xfId="370" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Normalny 13 3 3" xfId="371" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Normalny 13 3 3 2" xfId="372" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Normalny 13 3 3 2 2" xfId="373" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Normalny 13 3 3 3" xfId="374" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Normalny 13 3 4" xfId="375" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Normalny 13 3 4 2" xfId="376" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Normalny 13 3 5" xfId="377" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Normalny 13 4" xfId="378" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Normalny 13 4 2" xfId="379" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Normalny 13 4 2 2" xfId="380" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Normalny 13 4 2 2 2" xfId="381" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Normalny 13 4 2 3" xfId="382" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Normalny 13 4 3" xfId="383" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Normalny 13 4 3 2" xfId="384" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Normalny 13 4 4" xfId="385" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Normalny 13 5" xfId="386" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Normalny 13 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Normalny 13 5 2 2" xfId="388" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Normalny 13 5 3" xfId="389" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normalny 13 6" xfId="390" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normalny 13 6 2" xfId="391" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normalny 13 7" xfId="392" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Normalny 14" xfId="393" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Normalny 14 2" xfId="394" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Normalny 14 2 2" xfId="395" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Normalny 14 3" xfId="396" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Normalny 15" xfId="397" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Normalny 15 2" xfId="398" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Normalny 16" xfId="399" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Normalny 16 2" xfId="400" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Normalny 17" xfId="401" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Normalny 17 2" xfId="402" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Normalny 18" xfId="403" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Normalny 18 2" xfId="404" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Normalny 19" xfId="405" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Normalny 19 2" xfId="406" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Normalny 2 10" xfId="408" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Normalny 2 10 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Normalny 2 10 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Normalny 2 10 2 2 2" xfId="411" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Normalny 2 10 2 3" xfId="412" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Normalny 2 10 3" xfId="413" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Normalny 2 10 3 2" xfId="414" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Normalny 2 10 4" xfId="415" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Normalny 2 11" xfId="416" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Normalny 2 11 2" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Normalny 2 11 2 2" xfId="418" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Normalny 2 11 2 2 2" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Normalny 2 11 2 3" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Normalny 2 11 3" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Normalny 2 11 3 2" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Normalny 2 11 4" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Normalny 2 2" xfId="407" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Normalny 2 2 2" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Normalny 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Normalny 2 4" xfId="426" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Normalny 2 5" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normalny 2 6" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Normalny 2 7" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Normalny 2 7 2" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Normalny 2 7 2 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Normalny 2 7 2 2 2" xfId="432" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Normalny 2 7 2 2 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Normalny 2 7 2 2 3" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Normalny 2 7 2 3" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Normalny 2 7 2 3 2" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Normalny 2 7 2 4" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Normalny 2 7 3" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Normalny 2 7 3 2" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Normalny 2 7 3 2 2" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Normalny 2 7 3 3" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Normalny 2 7 4" xfId="442" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Normalny 2 7 4 2" xfId="443" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Normalny 2 7 5" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Normalny 2 8" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Normalny 2 8 2" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Normalny 2 8 2 2" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Normalny 2 8 2 2 2" xfId="448" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Normalny 2 8 2 2 2 2" xfId="449" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Normalny 2 8 2 2 3" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Normalny 2 8 2 3" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Normalny 2 8 2 3 2" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Normalny 2 8 2 4" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Normalny 2 8 3" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Normalny 2 8 3 2" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Normalny 2 8 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Normalny 2 8 3 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Normalny 2 8 4" xfId="458" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Normalny 2 8 4 2" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Normalny 2 8 5" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Normalny 2 9" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Normalny 20" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Normalny 20 2" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Normalny 21" xfId="464" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Normalny 21 2" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Normalny 22" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Normalny 22 2" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Normalny 23" xfId="468" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Normalny 23 2" xfId="469" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Normalny 24" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Normalny 24 2" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Normalny 25" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Normalny 25 2" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Normalny 26" xfId="474" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Normalny 26 2" xfId="475" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Normalny 27" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Normalny 27 2" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Normalny 28" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Normalny 28 2" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Normalny 29" xfId="480" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Normalny 29 2" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Normalny 3" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Normalny 3 2" xfId="483" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Normalny 3 2 2" xfId="484" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Normalny 3 2 3" xfId="485" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Normalny 3 2 4" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Normalny 3 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Normalny 3 4" xfId="488" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Normalny 3 4 2" xfId="489" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Normalny 3 4 2 2" xfId="490" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Normalny 3 4 3" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Normalny 3 5" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Normalny 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Normalny 3 6" xfId="494" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Normalny 30" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Normalny 30 2" xfId="496" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Normalny 31" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Normalny 31 2" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Normalny 32" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Normalny 32 2" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Normalny 33" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Normalny 33 2" xfId="502" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Normalny 34" xfId="503" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Normalny 34 2" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Normalny 35" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Normalny 35 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Normalny 36" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Normalny 36 2" xfId="508" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Normalny 37" xfId="509" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Normalny 37 2" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Normalny 38" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Normalny 38 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Normalny 39" xfId="513" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Normalny 39 2" xfId="514" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Normalny 4" xfId="515" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Normalny 4 2" xfId="516" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Normalny 4 3" xfId="517" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Normalny 40" xfId="518" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Normalny 40 2" xfId="519" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Normalny 41" xfId="520" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Normalny 41 2" xfId="521" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Normalny 42" xfId="522" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Normalny 42 2" xfId="523" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Normalny 43" xfId="524" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Normalny 43 2" xfId="525" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Normalny 44" xfId="526" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Normalny 44 2" xfId="527" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Normalny 45" xfId="528" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Normalny 45 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Normalny 46" xfId="530" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Normalny 46 2" xfId="531" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Normalny 47" xfId="532" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Normalny 47 2" xfId="533" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Normalny 48" xfId="534" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Normalny 48 2" xfId="535" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Normalny 49" xfId="536" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Normalny 49 2" xfId="537" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Normalny 5" xfId="538" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Normalny 5 2" xfId="539" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Normalny 50" xfId="540" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Normalny 50 2" xfId="541" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Normalny 51" xfId="542" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Normalny 51 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Normalny 52" xfId="544" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Normalny 52 2" xfId="545" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Normalny 53" xfId="546" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Normalny 53 2" xfId="547" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Normalny 54" xfId="548" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Normalny 54 2" xfId="549" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Normalny 55" xfId="550" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Normalny 56" xfId="551" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Normalny 56 2" xfId="552" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="Normalny 57" xfId="553" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normalny 57 2" xfId="554" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normalny 57 3" xfId="555" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normalny 58" xfId="556" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normalny 58 2" xfId="557" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normalny 59" xfId="558" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normalny 59 2" xfId="559" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normalny 59 3" xfId="560" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normalny 6" xfId="561" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normalny 6 2" xfId="562" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normalny 60" xfId="563" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normalny 60 2" xfId="564" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normalny 61" xfId="565" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normalny 61 2" xfId="566" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normalny 61 3" xfId="567" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normalny 62" xfId="568" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normalny 62 2" xfId="569" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normalny 63" xfId="570" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normalny 63 2" xfId="571" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normalny 64" xfId="572" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normalny 64 2" xfId="573" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normalny 65" xfId="574" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normalny 66" xfId="575" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normalny 67" xfId="576" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normalny 68" xfId="577" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normalny 68 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normalny 68 2 2" xfId="579" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normalny 68 3" xfId="580" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normalny 69" xfId="581" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normalny 69 2" xfId="582" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normalny 7" xfId="583" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normalny 7 2" xfId="584" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normalny 70" xfId="585" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normalny 70 2" xfId="586" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normalny 70 2 2" xfId="587" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normalny 70 2 2 2" xfId="588" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normalny 70 2 2 2 2" xfId="589" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normalny 70 2 2 2 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normalny 70 2 2 2 3" xfId="591" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normalny 70 2 2 3" xfId="592" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normalny 70 2 2 3 2" xfId="593" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normalny 70 2 2 4" xfId="594" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normalny 70 2 3" xfId="595" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normalny 70 2 3 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normalny 70 2 3 2 2" xfId="597" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normalny 70 2 3 3" xfId="598" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normalny 70 2 4" xfId="599" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normalny 70 2 4 2" xfId="600" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normalny 70 2 5" xfId="601" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normalny 70 3" xfId="602" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normalny 70 3 2" xfId="603" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normalny 70 3 2 2" xfId="604" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normalny 70 3 2 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normalny 70 3 2 2 2 2" xfId="606" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normalny 70 3 2 2 3" xfId="607" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normalny 70 3 2 3" xfId="608" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normalny 70 3 2 3 2" xfId="609" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normalny 70 3 2 4" xfId="610" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normalny 70 3 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normalny 70 3 3 2" xfId="612" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normalny 70 3 3 2 2" xfId="613" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normalny 70 3 3 3" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normalny 70 3 4" xfId="615" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normalny 70 3 4 2" xfId="616" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normalny 70 3 5" xfId="617" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normalny 70 4" xfId="618" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normalny 70 4 2" xfId="619" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normalny 70 4 2 2" xfId="620" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normalny 70 4 2 2 2" xfId="621" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normalny 70 4 2 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normalny 70 4 3" xfId="623" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normalny 70 4 3 2" xfId="624" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normalny 70 4 4" xfId="625" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normalny 70 5" xfId="626" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normalny 70 5 2" xfId="627" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normalny 70 5 2 2" xfId="628" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normalny 70 5 3" xfId="629" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normalny 70 6" xfId="630" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normalny 70 6 2" xfId="631" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normalny 70 7" xfId="632" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normalny 71" xfId="633" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normalny 71 2" xfId="634" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normalny 71 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normalny 71 2 2 2" xfId="636" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normalny 71 2 2 2 2" xfId="637" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normalny 71 2 2 2 2 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normalny 71 2 2 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normalny 71 2 2 3" xfId="640" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normalny 71 2 2 3 2" xfId="641" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normalny 71 2 2 4" xfId="642" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normalny 71 2 3" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normalny 71 2 3 2" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normalny 71 2 3 2 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normalny 71 2 3 3" xfId="646" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normalny 71 2 4" xfId="647" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normalny 71 2 4 2" xfId="648" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normalny 71 2 5" xfId="649" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normalny 71 3" xfId="650" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normalny 71 3 2" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normalny 71 3 2 2" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normalny 71 3 2 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normalny 71 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normalny 71 3 3" xfId="655" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Normalny 71 3 3 2" xfId="656" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Normalny 71 3 4" xfId="657" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Normalny 71 4" xfId="658" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Normalny 71 4 2" xfId="659" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Normalny 71 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Normalny 71 4 3" xfId="661" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Normalny 71 5" xfId="662" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="Normalny 71 5 2" xfId="663" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
+    <cellStyle name="Normalny 71 6" xfId="664" xr:uid="{00000000-0005-0000-0000-000098020000}"/>
+    <cellStyle name="Normalny 72" xfId="665" xr:uid="{00000000-0005-0000-0000-000099020000}"/>
+    <cellStyle name="Normalny 72 2" xfId="666" xr:uid="{00000000-0005-0000-0000-00009A020000}"/>
+    <cellStyle name="Normalny 72 2 2" xfId="667" xr:uid="{00000000-0005-0000-0000-00009B020000}"/>
+    <cellStyle name="Normalny 72 2 2 2" xfId="668" xr:uid="{00000000-0005-0000-0000-00009C020000}"/>
+    <cellStyle name="Normalny 72 2 2 2 2" xfId="669" xr:uid="{00000000-0005-0000-0000-00009D020000}"/>
+    <cellStyle name="Normalny 72 2 2 2 2 2" xfId="670" xr:uid="{00000000-0005-0000-0000-00009E020000}"/>
+    <cellStyle name="Normalny 72 2 2 2 3" xfId="671" xr:uid="{00000000-0005-0000-0000-00009F020000}"/>
+    <cellStyle name="Normalny 72 2 2 3" xfId="672" xr:uid="{00000000-0005-0000-0000-0000A0020000}"/>
+    <cellStyle name="Normalny 72 2 2 3 2" xfId="673" xr:uid="{00000000-0005-0000-0000-0000A1020000}"/>
+    <cellStyle name="Normalny 72 2 2 4" xfId="674" xr:uid="{00000000-0005-0000-0000-0000A2020000}"/>
+    <cellStyle name="Normalny 72 2 3" xfId="675" xr:uid="{00000000-0005-0000-0000-0000A3020000}"/>
+    <cellStyle name="Normalny 72 2 3 2" xfId="676" xr:uid="{00000000-0005-0000-0000-0000A4020000}"/>
+    <cellStyle name="Normalny 72 2 3 2 2" xfId="677" xr:uid="{00000000-0005-0000-0000-0000A5020000}"/>
+    <cellStyle name="Normalny 72 2 3 3" xfId="678" xr:uid="{00000000-0005-0000-0000-0000A6020000}"/>
+    <cellStyle name="Normalny 72 2 4" xfId="679" xr:uid="{00000000-0005-0000-0000-0000A7020000}"/>
+    <cellStyle name="Normalny 72 2 4 2" xfId="680" xr:uid="{00000000-0005-0000-0000-0000A8020000}"/>
+    <cellStyle name="Normalny 72 2 5" xfId="681" xr:uid="{00000000-0005-0000-0000-0000A9020000}"/>
+    <cellStyle name="Normalny 72 3" xfId="682" xr:uid="{00000000-0005-0000-0000-0000AA020000}"/>
+    <cellStyle name="Normalny 72 3 2" xfId="683" xr:uid="{00000000-0005-0000-0000-0000AB020000}"/>
+    <cellStyle name="Normalny 72 3 2 2" xfId="684" xr:uid="{00000000-0005-0000-0000-0000AC020000}"/>
+    <cellStyle name="Normalny 72 3 2 2 2" xfId="685" xr:uid="{00000000-0005-0000-0000-0000AD020000}"/>
+    <cellStyle name="Normalny 72 3 2 3" xfId="686" xr:uid="{00000000-0005-0000-0000-0000AE020000}"/>
+    <cellStyle name="Normalny 72 3 3" xfId="687" xr:uid="{00000000-0005-0000-0000-0000AF020000}"/>
+    <cellStyle name="Normalny 72 3 3 2" xfId="688" xr:uid="{00000000-0005-0000-0000-0000B0020000}"/>
+    <cellStyle name="Normalny 72 3 4" xfId="689" xr:uid="{00000000-0005-0000-0000-0000B1020000}"/>
+    <cellStyle name="Normalny 72 4" xfId="690" xr:uid="{00000000-0005-0000-0000-0000B2020000}"/>
+    <cellStyle name="Normalny 72 4 2" xfId="691" xr:uid="{00000000-0005-0000-0000-0000B3020000}"/>
+    <cellStyle name="Normalny 72 4 2 2" xfId="692" xr:uid="{00000000-0005-0000-0000-0000B4020000}"/>
+    <cellStyle name="Normalny 72 4 3" xfId="693" xr:uid="{00000000-0005-0000-0000-0000B5020000}"/>
+    <cellStyle name="Normalny 72 5" xfId="694" xr:uid="{00000000-0005-0000-0000-0000B6020000}"/>
+    <cellStyle name="Normalny 72 5 2" xfId="695" xr:uid="{00000000-0005-0000-0000-0000B7020000}"/>
+    <cellStyle name="Normalny 72 6" xfId="696" xr:uid="{00000000-0005-0000-0000-0000B8020000}"/>
+    <cellStyle name="Normalny 73" xfId="697" xr:uid="{00000000-0005-0000-0000-0000B9020000}"/>
+    <cellStyle name="Normalny 73 2" xfId="698" xr:uid="{00000000-0005-0000-0000-0000BA020000}"/>
+    <cellStyle name="Normalny 73 2 2" xfId="699" xr:uid="{00000000-0005-0000-0000-0000BB020000}"/>
+    <cellStyle name="Normalny 73 2 2 2" xfId="700" xr:uid="{00000000-0005-0000-0000-0000BC020000}"/>
+    <cellStyle name="Normalny 73 2 2 2 2" xfId="701" xr:uid="{00000000-0005-0000-0000-0000BD020000}"/>
+    <cellStyle name="Normalny 73 2 2 2 2 2" xfId="702" xr:uid="{00000000-0005-0000-0000-0000BE020000}"/>
+    <cellStyle name="Normalny 73 2 2 2 3" xfId="703" xr:uid="{00000000-0005-0000-0000-0000BF020000}"/>
+    <cellStyle name="Normalny 73 2 2 3" xfId="704" xr:uid="{00000000-0005-0000-0000-0000C0020000}"/>
+    <cellStyle name="Normalny 73 2 2 3 2" xfId="705" xr:uid="{00000000-0005-0000-0000-0000C1020000}"/>
+    <cellStyle name="Normalny 73 2 2 4" xfId="706" xr:uid="{00000000-0005-0000-0000-0000C2020000}"/>
+    <cellStyle name="Normalny 73 2 3" xfId="707" xr:uid="{00000000-0005-0000-0000-0000C3020000}"/>
+    <cellStyle name="Normalny 73 2 3 2" xfId="708" xr:uid="{00000000-0005-0000-0000-0000C4020000}"/>
+    <cellStyle name="Normalny 73 2 3 2 2" xfId="709" xr:uid="{00000000-0005-0000-0000-0000C5020000}"/>
+    <cellStyle name="Normalny 73 2 3 3" xfId="710" xr:uid="{00000000-0005-0000-0000-0000C6020000}"/>
+    <cellStyle name="Normalny 73 2 4" xfId="711" xr:uid="{00000000-0005-0000-0000-0000C7020000}"/>
+    <cellStyle name="Normalny 73 2 4 2" xfId="712" xr:uid="{00000000-0005-0000-0000-0000C8020000}"/>
+    <cellStyle name="Normalny 73 2 5" xfId="713" xr:uid="{00000000-0005-0000-0000-0000C9020000}"/>
+    <cellStyle name="Normalny 73 3" xfId="714" xr:uid="{00000000-0005-0000-0000-0000CA020000}"/>
+    <cellStyle name="Normalny 73 3 2" xfId="715" xr:uid="{00000000-0005-0000-0000-0000CB020000}"/>
+    <cellStyle name="Normalny 73 3 2 2" xfId="716" xr:uid="{00000000-0005-0000-0000-0000CC020000}"/>
+    <cellStyle name="Normalny 73 3 2 2 2" xfId="717" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
+    <cellStyle name="Normalny 73 3 2 3" xfId="718" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
+    <cellStyle name="Normalny 73 3 3" xfId="719" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
+    <cellStyle name="Normalny 73 3 3 2" xfId="720" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
+    <cellStyle name="Normalny 73 3 4" xfId="721" xr:uid="{00000000-0005-0000-0000-0000D1020000}"/>
+    <cellStyle name="Normalny 73 4" xfId="722" xr:uid="{00000000-0005-0000-0000-0000D2020000}"/>
+    <cellStyle name="Normalny 73 4 2" xfId="723" xr:uid="{00000000-0005-0000-0000-0000D3020000}"/>
+    <cellStyle name="Normalny 73 4 2 2" xfId="724" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Normalny 73 4 3" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normalny 73 5" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
+    <cellStyle name="Normalny 73 5 2" xfId="727" xr:uid="{00000000-0005-0000-0000-0000D7020000}"/>
+    <cellStyle name="Normalny 73 6" xfId="728" xr:uid="{00000000-0005-0000-0000-0000D8020000}"/>
+    <cellStyle name="Normalny 74" xfId="729" xr:uid="{00000000-0005-0000-0000-0000D9020000}"/>
+    <cellStyle name="Normalny 74 2" xfId="730" xr:uid="{00000000-0005-0000-0000-0000DA020000}"/>
+    <cellStyle name="Normalny 74 2 2" xfId="731" xr:uid="{00000000-0005-0000-0000-0000DB020000}"/>
+    <cellStyle name="Normalny 74 2 2 2" xfId="732" xr:uid="{00000000-0005-0000-0000-0000DC020000}"/>
+    <cellStyle name="Normalny 74 2 2 2 2" xfId="733" xr:uid="{00000000-0005-0000-0000-0000DD020000}"/>
+    <cellStyle name="Normalny 74 2 2 2 2 2" xfId="734" xr:uid="{00000000-0005-0000-0000-0000DE020000}"/>
+    <cellStyle name="Normalny 74 2 2 2 3" xfId="735" xr:uid="{00000000-0005-0000-0000-0000DF020000}"/>
+    <cellStyle name="Normalny 74 2 2 3" xfId="736" xr:uid="{00000000-0005-0000-0000-0000E0020000}"/>
+    <cellStyle name="Normalny 74 2 2 3 2" xfId="737" xr:uid="{00000000-0005-0000-0000-0000E1020000}"/>
+    <cellStyle name="Normalny 74 2 2 4" xfId="738" xr:uid="{00000000-0005-0000-0000-0000E2020000}"/>
+    <cellStyle name="Normalny 74 2 3" xfId="739" xr:uid="{00000000-0005-0000-0000-0000E3020000}"/>
+    <cellStyle name="Normalny 74 2 3 2" xfId="740" xr:uid="{00000000-0005-0000-0000-0000E4020000}"/>
+    <cellStyle name="Normalny 74 2 3 2 2" xfId="741" xr:uid="{00000000-0005-0000-0000-0000E5020000}"/>
+    <cellStyle name="Normalny 74 2 3 3" xfId="742" xr:uid="{00000000-0005-0000-0000-0000E6020000}"/>
+    <cellStyle name="Normalny 74 2 4" xfId="743" xr:uid="{00000000-0005-0000-0000-0000E7020000}"/>
+    <cellStyle name="Normalny 74 2 4 2" xfId="744" xr:uid="{00000000-0005-0000-0000-0000E8020000}"/>
+    <cellStyle name="Normalny 74 2 5" xfId="745" xr:uid="{00000000-0005-0000-0000-0000E9020000}"/>
+    <cellStyle name="Normalny 74 3" xfId="746" xr:uid="{00000000-0005-0000-0000-0000EA020000}"/>
+    <cellStyle name="Normalny 74 3 2" xfId="747" xr:uid="{00000000-0005-0000-0000-0000EB020000}"/>
+    <cellStyle name="Normalny 74 3 2 2" xfId="748" xr:uid="{00000000-0005-0000-0000-0000EC020000}"/>
+    <cellStyle name="Normalny 74 3 2 2 2" xfId="749" xr:uid="{00000000-0005-0000-0000-0000ED020000}"/>
+    <cellStyle name="Normalny 74 3 2 3" xfId="750" xr:uid="{00000000-0005-0000-0000-0000EE020000}"/>
+    <cellStyle name="Normalny 74 3 3" xfId="751" xr:uid="{00000000-0005-0000-0000-0000EF020000}"/>
+    <cellStyle name="Normalny 74 3 3 2" xfId="752" xr:uid="{00000000-0005-0000-0000-0000F0020000}"/>
+    <cellStyle name="Normalny 74 3 4" xfId="753" xr:uid="{00000000-0005-0000-0000-0000F1020000}"/>
+    <cellStyle name="Normalny 74 4" xfId="754" xr:uid="{00000000-0005-0000-0000-0000F2020000}"/>
+    <cellStyle name="Normalny 74 4 2" xfId="755" xr:uid="{00000000-0005-0000-0000-0000F3020000}"/>
+    <cellStyle name="Normalny 74 4 2 2" xfId="756" xr:uid="{00000000-0005-0000-0000-0000F4020000}"/>
+    <cellStyle name="Normalny 74 4 3" xfId="757" xr:uid="{00000000-0005-0000-0000-0000F5020000}"/>
+    <cellStyle name="Normalny 74 5" xfId="758" xr:uid="{00000000-0005-0000-0000-0000F6020000}"/>
+    <cellStyle name="Normalny 74 5 2" xfId="759" xr:uid="{00000000-0005-0000-0000-0000F7020000}"/>
+    <cellStyle name="Normalny 74 6" xfId="760" xr:uid="{00000000-0005-0000-0000-0000F8020000}"/>
+    <cellStyle name="Normalny 75" xfId="761" xr:uid="{00000000-0005-0000-0000-0000F9020000}"/>
+    <cellStyle name="Normalny 75 2" xfId="762" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
+    <cellStyle name="Normalny 75 2 2" xfId="763" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
+    <cellStyle name="Normalny 75 2 2 2" xfId="764" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
+    <cellStyle name="Normalny 75 2 3" xfId="765" xr:uid="{00000000-0005-0000-0000-0000FD020000}"/>
+    <cellStyle name="Normalny 75 3" xfId="766" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
+    <cellStyle name="Normalny 75 3 2" xfId="767" xr:uid="{00000000-0005-0000-0000-0000FF020000}"/>
+    <cellStyle name="Normalny 75 4" xfId="768" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
+    <cellStyle name="Normalny 76" xfId="769" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
+    <cellStyle name="Normalny 77" xfId="770" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
+    <cellStyle name="Normalny 77 2" xfId="771" xr:uid="{00000000-0005-0000-0000-000003030000}"/>
+    <cellStyle name="Normalny 77 2 2" xfId="772" xr:uid="{00000000-0005-0000-0000-000004030000}"/>
+    <cellStyle name="Normalny 77 3" xfId="773" xr:uid="{00000000-0005-0000-0000-000005030000}"/>
+    <cellStyle name="Normalny 78" xfId="774" xr:uid="{00000000-0005-0000-0000-000006030000}"/>
+    <cellStyle name="Normalny 79" xfId="775" xr:uid="{00000000-0005-0000-0000-000007030000}"/>
+    <cellStyle name="Normalny 79 2" xfId="776" xr:uid="{00000000-0005-0000-0000-000008030000}"/>
+    <cellStyle name="Normalny 8" xfId="777" xr:uid="{00000000-0005-0000-0000-000009030000}"/>
+    <cellStyle name="Normalny 8 2" xfId="778" xr:uid="{00000000-0005-0000-0000-00000A030000}"/>
+    <cellStyle name="Normalny 80" xfId="779" xr:uid="{00000000-0005-0000-0000-00000B030000}"/>
+    <cellStyle name="Normalny 81" xfId="780" xr:uid="{00000000-0005-0000-0000-00000C030000}"/>
+    <cellStyle name="Normalny 9" xfId="781" xr:uid="{00000000-0005-0000-0000-00000D030000}"/>
+    <cellStyle name="Normalny 9 2" xfId="782" xr:uid="{00000000-0005-0000-0000-00000E030000}"/>
+    <cellStyle name="Opis" xfId="783" xr:uid="{00000000-0005-0000-0000-00000F030000}"/>
+    <cellStyle name="Percent [2]" xfId="784" xr:uid="{00000000-0005-0000-0000-000010030000}"/>
+    <cellStyle name="Percent [2] 2" xfId="785" xr:uid="{00000000-0005-0000-0000-000011030000}"/>
+    <cellStyle name="Percent 2" xfId="786" xr:uid="{00000000-0005-0000-0000-000012030000}"/>
+    <cellStyle name="Percent 2 2" xfId="787" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
+    <cellStyle name="Percent 2 2 2" xfId="788" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
+    <cellStyle name="Percent 2 3" xfId="789" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
+    <cellStyle name="Percent 2 3 2" xfId="790" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
+    <cellStyle name="Percent 2 3 2 2" xfId="791" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
+    <cellStyle name="Percent 2 3 2 2 2" xfId="792" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
+    <cellStyle name="Percent 2 3 2 2 2 2" xfId="793" xr:uid="{00000000-0005-0000-0000-000019030000}"/>
+    <cellStyle name="Percent 2 3 2 2 3" xfId="794" xr:uid="{00000000-0005-0000-0000-00001A030000}"/>
+    <cellStyle name="Percent 2 3 2 3" xfId="795" xr:uid="{00000000-0005-0000-0000-00001B030000}"/>
+    <cellStyle name="Percent 2 3 2 3 2" xfId="796" xr:uid="{00000000-0005-0000-0000-00001C030000}"/>
+    <cellStyle name="Percent 2 3 2 4" xfId="797" xr:uid="{00000000-0005-0000-0000-00001D030000}"/>
+    <cellStyle name="Percent 2 3 3" xfId="798" xr:uid="{00000000-0005-0000-0000-00001E030000}"/>
+    <cellStyle name="Percent 2 3 3 2" xfId="799" xr:uid="{00000000-0005-0000-0000-00001F030000}"/>
+    <cellStyle name="Percent 2 3 3 2 2" xfId="800" xr:uid="{00000000-0005-0000-0000-000020030000}"/>
+    <cellStyle name="Percent 2 3 3 3" xfId="801" xr:uid="{00000000-0005-0000-0000-000021030000}"/>
+    <cellStyle name="Percent 2 3 4" xfId="802" xr:uid="{00000000-0005-0000-0000-000022030000}"/>
+    <cellStyle name="Percent 2 3 4 2" xfId="803" xr:uid="{00000000-0005-0000-0000-000023030000}"/>
+    <cellStyle name="Percent 2 3 5" xfId="804" xr:uid="{00000000-0005-0000-0000-000024030000}"/>
+    <cellStyle name="Percent 2 4" xfId="805" xr:uid="{00000000-0005-0000-0000-000025030000}"/>
+    <cellStyle name="Percent 2 4 2" xfId="806" xr:uid="{00000000-0005-0000-0000-000026030000}"/>
+    <cellStyle name="Percent 2 4 2 2" xfId="807" xr:uid="{00000000-0005-0000-0000-000027030000}"/>
+    <cellStyle name="Percent 2 4 2 2 2" xfId="808" xr:uid="{00000000-0005-0000-0000-000028030000}"/>
+    <cellStyle name="Percent 2 4 2 2 2 2" xfId="809" xr:uid="{00000000-0005-0000-0000-000029030000}"/>
+    <cellStyle name="Percent 2 4 2 2 3" xfId="810" xr:uid="{00000000-0005-0000-0000-00002A030000}"/>
+    <cellStyle name="Percent 2 4 2 3" xfId="811" xr:uid="{00000000-0005-0000-0000-00002B030000}"/>
+    <cellStyle name="Percent 2 4 2 3 2" xfId="812" xr:uid="{00000000-0005-0000-0000-00002C030000}"/>
+    <cellStyle name="Percent 2 4 2 4" xfId="813" xr:uid="{00000000-0005-0000-0000-00002D030000}"/>
+    <cellStyle name="Percent 2 4 3" xfId="814" xr:uid="{00000000-0005-0000-0000-00002E030000}"/>
+    <cellStyle name="Percent 2 4 3 2" xfId="815" xr:uid="{00000000-0005-0000-0000-00002F030000}"/>
+    <cellStyle name="Percent 2 4 3 2 2" xfId="816" xr:uid="{00000000-0005-0000-0000-000030030000}"/>
+    <cellStyle name="Percent 2 4 3 3" xfId="817" xr:uid="{00000000-0005-0000-0000-000031030000}"/>
+    <cellStyle name="Percent 2 4 4" xfId="818" xr:uid="{00000000-0005-0000-0000-000032030000}"/>
+    <cellStyle name="Percent 2 4 4 2" xfId="819" xr:uid="{00000000-0005-0000-0000-000033030000}"/>
+    <cellStyle name="Percent 2 4 5" xfId="820" xr:uid="{00000000-0005-0000-0000-000034030000}"/>
+    <cellStyle name="Percent 2 5" xfId="821" xr:uid="{00000000-0005-0000-0000-000035030000}"/>
+    <cellStyle name="Percent 2 5 2" xfId="822" xr:uid="{00000000-0005-0000-0000-000036030000}"/>
+    <cellStyle name="Percent 2 5 2 2" xfId="823" xr:uid="{00000000-0005-0000-0000-000037030000}"/>
+    <cellStyle name="Percent 2 5 2 2 2" xfId="824" xr:uid="{00000000-0005-0000-0000-000038030000}"/>
+    <cellStyle name="Percent 2 5 2 3" xfId="825" xr:uid="{00000000-0005-0000-0000-000039030000}"/>
+    <cellStyle name="Percent 2 5 3" xfId="826" xr:uid="{00000000-0005-0000-0000-00003A030000}"/>
+    <cellStyle name="Percent 2 5 3 2" xfId="827" xr:uid="{00000000-0005-0000-0000-00003B030000}"/>
+    <cellStyle name="Percent 2 5 4" xfId="828" xr:uid="{00000000-0005-0000-0000-00003C030000}"/>
+    <cellStyle name="Percent 2 6" xfId="829" xr:uid="{00000000-0005-0000-0000-00003D030000}"/>
+    <cellStyle name="Percent 2 6 2" xfId="830" xr:uid="{00000000-0005-0000-0000-00003E030000}"/>
+    <cellStyle name="Percent 2 6 2 2" xfId="831" xr:uid="{00000000-0005-0000-0000-00003F030000}"/>
+    <cellStyle name="Percent 2 6 3" xfId="832" xr:uid="{00000000-0005-0000-0000-000040030000}"/>
+    <cellStyle name="Percent 2 7" xfId="833" xr:uid="{00000000-0005-0000-0000-000041030000}"/>
+    <cellStyle name="Percent 2 7 2" xfId="834" xr:uid="{00000000-0005-0000-0000-000042030000}"/>
+    <cellStyle name="Percent 2 8" xfId="835" xr:uid="{00000000-0005-0000-0000-000043030000}"/>
+    <cellStyle name="Percent 3" xfId="836" xr:uid="{00000000-0005-0000-0000-000044030000}"/>
+    <cellStyle name="Percent 3 2" xfId="837" xr:uid="{00000000-0005-0000-0000-000045030000}"/>
+    <cellStyle name="Percent 3 2 2" xfId="838" xr:uid="{00000000-0005-0000-0000-000046030000}"/>
+    <cellStyle name="Percent 3 2 2 2" xfId="839" xr:uid="{00000000-0005-0000-0000-000047030000}"/>
+    <cellStyle name="Percent 3 2 2 2 2" xfId="840" xr:uid="{00000000-0005-0000-0000-000048030000}"/>
+    <cellStyle name="Percent 3 2 2 2 2 2" xfId="841" xr:uid="{00000000-0005-0000-0000-000049030000}"/>
+    <cellStyle name="Percent 3 2 2 2 3" xfId="842" xr:uid="{00000000-0005-0000-0000-00004A030000}"/>
+    <cellStyle name="Percent 3 2 2 3" xfId="843" xr:uid="{00000000-0005-0000-0000-00004B030000}"/>
+    <cellStyle name="Percent 3 2 2 3 2" xfId="844" xr:uid="{00000000-0005-0000-0000-00004C030000}"/>
+    <cellStyle name="Percent 3 2 2 4" xfId="845" xr:uid="{00000000-0005-0000-0000-00004D030000}"/>
+    <cellStyle name="Percent 3 2 3" xfId="846" xr:uid="{00000000-0005-0000-0000-00004E030000}"/>
+    <cellStyle name="Percent 3 2 3 2" xfId="847" xr:uid="{00000000-0005-0000-0000-00004F030000}"/>
+    <cellStyle name="Percent 3 2 3 2 2" xfId="848" xr:uid="{00000000-0005-0000-0000-000050030000}"/>
+    <cellStyle name="Percent 3 2 3 3" xfId="849" xr:uid="{00000000-0005-0000-0000-000051030000}"/>
+    <cellStyle name="Percent 3 2 4" xfId="850" xr:uid="{00000000-0005-0000-0000-000052030000}"/>
+    <cellStyle name="Percent 3 2 4 2" xfId="851" xr:uid="{00000000-0005-0000-0000-000053030000}"/>
+    <cellStyle name="Percent 3 2 5" xfId="852" xr:uid="{00000000-0005-0000-0000-000054030000}"/>
+    <cellStyle name="Percent 3 3" xfId="853" xr:uid="{00000000-0005-0000-0000-000055030000}"/>
+    <cellStyle name="Percent 3 3 2" xfId="854" xr:uid="{00000000-0005-0000-0000-000056030000}"/>
+    <cellStyle name="Percent 3 3 2 2" xfId="855" xr:uid="{00000000-0005-0000-0000-000057030000}"/>
+    <cellStyle name="Percent 3 3 2 2 2" xfId="856" xr:uid="{00000000-0005-0000-0000-000058030000}"/>
+    <cellStyle name="Percent 3 3 2 2 2 2" xfId="857" xr:uid="{00000000-0005-0000-0000-000059030000}"/>
+    <cellStyle name="Percent 3 3 2 2 3" xfId="858" xr:uid="{00000000-0005-0000-0000-00005A030000}"/>
+    <cellStyle name="Percent 3 3 2 3" xfId="859" xr:uid="{00000000-0005-0000-0000-00005B030000}"/>
+    <cellStyle name="Percent 3 3 2 3 2" xfId="860" xr:uid="{00000000-0005-0000-0000-00005C030000}"/>
+    <cellStyle name="Percent 3 3 2 4" xfId="861" xr:uid="{00000000-0005-0000-0000-00005D030000}"/>
+    <cellStyle name="Percent 3 3 3" xfId="862" xr:uid="{00000000-0005-0000-0000-00005E030000}"/>
+    <cellStyle name="Percent 3 3 3 2" xfId="863" xr:uid="{00000000-0005-0000-0000-00005F030000}"/>
+    <cellStyle name="Percent 3 3 3 2 2" xfId="864" xr:uid="{00000000-0005-0000-0000-000060030000}"/>
+    <cellStyle name="Percent 3 3 3 3" xfId="865" xr:uid="{00000000-0005-0000-0000-000061030000}"/>
+    <cellStyle name="Percent 3 3 4" xfId="866" xr:uid="{00000000-0005-0000-0000-000062030000}"/>
+    <cellStyle name="Percent 3 3 4 2" xfId="867" xr:uid="{00000000-0005-0000-0000-000063030000}"/>
+    <cellStyle name="Percent 3 3 5" xfId="868" xr:uid="{00000000-0005-0000-0000-000064030000}"/>
+    <cellStyle name="Percent 3 4" xfId="869" xr:uid="{00000000-0005-0000-0000-000065030000}"/>
+    <cellStyle name="Percent 3 4 2" xfId="870" xr:uid="{00000000-0005-0000-0000-000066030000}"/>
+    <cellStyle name="Percent 3 4 2 2" xfId="871" xr:uid="{00000000-0005-0000-0000-000067030000}"/>
+    <cellStyle name="Percent 3 4 2 2 2" xfId="872" xr:uid="{00000000-0005-0000-0000-000068030000}"/>
+    <cellStyle name="Percent 3 4 2 3" xfId="873" xr:uid="{00000000-0005-0000-0000-000069030000}"/>
+    <cellStyle name="Percent 3 4 3" xfId="874" xr:uid="{00000000-0005-0000-0000-00006A030000}"/>
+    <cellStyle name="Percent 3 4 3 2" xfId="875" xr:uid="{00000000-0005-0000-0000-00006B030000}"/>
+    <cellStyle name="Percent 3 4 4" xfId="876" xr:uid="{00000000-0005-0000-0000-00006C030000}"/>
+    <cellStyle name="Percent 3 5" xfId="877" xr:uid="{00000000-0005-0000-0000-00006D030000}"/>
+    <cellStyle name="Percent 3 5 2" xfId="878" xr:uid="{00000000-0005-0000-0000-00006E030000}"/>
+    <cellStyle name="Percent 3 5 2 2" xfId="879" xr:uid="{00000000-0005-0000-0000-00006F030000}"/>
+    <cellStyle name="Percent 3 5 3" xfId="880" xr:uid="{00000000-0005-0000-0000-000070030000}"/>
+    <cellStyle name="Percent 3 6" xfId="881" xr:uid="{00000000-0005-0000-0000-000071030000}"/>
+    <cellStyle name="Percent 3 6 2" xfId="882" xr:uid="{00000000-0005-0000-0000-000072030000}"/>
+    <cellStyle name="Percent 3 7" xfId="883" xr:uid="{00000000-0005-0000-0000-000073030000}"/>
+    <cellStyle name="Procentowy 2" xfId="884" xr:uid="{00000000-0005-0000-0000-000074030000}"/>
+    <cellStyle name="Procentowy 2 2" xfId="885" xr:uid="{00000000-0005-0000-0000-000075030000}"/>
+    <cellStyle name="Procentowy 2 2 2" xfId="886" xr:uid="{00000000-0005-0000-0000-000076030000}"/>
+    <cellStyle name="Procentowy 2 3" xfId="887" xr:uid="{00000000-0005-0000-0000-000077030000}"/>
+    <cellStyle name="Procentowy 2 3 2" xfId="888" xr:uid="{00000000-0005-0000-0000-000078030000}"/>
+    <cellStyle name="Procentowy 2 3 2 2" xfId="889" xr:uid="{00000000-0005-0000-0000-000079030000}"/>
+    <cellStyle name="Procentowy 2 4" xfId="890" xr:uid="{00000000-0005-0000-0000-00007A030000}"/>
+    <cellStyle name="Procentowy 2 5" xfId="891" xr:uid="{00000000-0005-0000-0000-00007B030000}"/>
+    <cellStyle name="Procentowy 3" xfId="892" xr:uid="{00000000-0005-0000-0000-00007C030000}"/>
+    <cellStyle name="Procentowy 3 2" xfId="893" xr:uid="{00000000-0005-0000-0000-00007D030000}"/>
+    <cellStyle name="Procentowy 3 2 2" xfId="894" xr:uid="{00000000-0005-0000-0000-00007E030000}"/>
+    <cellStyle name="Procentowy 3 2 2 2" xfId="895" xr:uid="{00000000-0005-0000-0000-00007F030000}"/>
+    <cellStyle name="Procentowy 3 2 2 2 2" xfId="896" xr:uid="{00000000-0005-0000-0000-000080030000}"/>
+    <cellStyle name="Procentowy 3 2 2 2 2 2" xfId="897" xr:uid="{00000000-0005-0000-0000-000081030000}"/>
+    <cellStyle name="Procentowy 3 2 2 2 3" xfId="898" xr:uid="{00000000-0005-0000-0000-000082030000}"/>
+    <cellStyle name="Procentowy 3 2 2 3" xfId="899" xr:uid="{00000000-0005-0000-0000-000083030000}"/>
+    <cellStyle name="Procentowy 3 2 2 3 2" xfId="900" xr:uid="{00000000-0005-0000-0000-000084030000}"/>
+    <cellStyle name="Procentowy 3 2 2 4" xfId="901" xr:uid="{00000000-0005-0000-0000-000085030000}"/>
+    <cellStyle name="Procentowy 3 2 3" xfId="902" xr:uid="{00000000-0005-0000-0000-000086030000}"/>
+    <cellStyle name="Procentowy 3 2 3 2" xfId="903" xr:uid="{00000000-0005-0000-0000-000087030000}"/>
+    <cellStyle name="Procentowy 3 2 3 2 2" xfId="904" xr:uid="{00000000-0005-0000-0000-000088030000}"/>
+    <cellStyle name="Procentowy 3 2 3 3" xfId="905" xr:uid="{00000000-0005-0000-0000-000089030000}"/>
+    <cellStyle name="Procentowy 3 2 4" xfId="906" xr:uid="{00000000-0005-0000-0000-00008A030000}"/>
+    <cellStyle name="Procentowy 3 2 4 2" xfId="907" xr:uid="{00000000-0005-0000-0000-00008B030000}"/>
+    <cellStyle name="Procentowy 3 2 5" xfId="908" xr:uid="{00000000-0005-0000-0000-00008C030000}"/>
+    <cellStyle name="Procentowy 3 3" xfId="909" xr:uid="{00000000-0005-0000-0000-00008D030000}"/>
+    <cellStyle name="Procentowy 3 3 2" xfId="910" xr:uid="{00000000-0005-0000-0000-00008E030000}"/>
+    <cellStyle name="Procentowy 3 3 2 2" xfId="911" xr:uid="{00000000-0005-0000-0000-00008F030000}"/>
+    <cellStyle name="Procentowy 3 3 2 2 2" xfId="912" xr:uid="{00000000-0005-0000-0000-000090030000}"/>
+    <cellStyle name="Procentowy 3 3 2 2 2 2" xfId="913" xr:uid="{00000000-0005-0000-0000-000091030000}"/>
+    <cellStyle name="Procentowy 3 3 2 2 3" xfId="914" xr:uid="{00000000-0005-0000-0000-000092030000}"/>
+    <cellStyle name="Procentowy 3 3 2 3" xfId="915" xr:uid="{00000000-0005-0000-0000-000093030000}"/>
+    <cellStyle name="Procentowy 3 3 2 3 2" xfId="916" xr:uid="{00000000-0005-0000-0000-000094030000}"/>
+    <cellStyle name="Procentowy 3 3 2 4" xfId="917" xr:uid="{00000000-0005-0000-0000-000095030000}"/>
+    <cellStyle name="Procentowy 3 3 3" xfId="918" xr:uid="{00000000-0005-0000-0000-000096030000}"/>
+    <cellStyle name="Procentowy 3 3 3 2" xfId="919" xr:uid="{00000000-0005-0000-0000-000097030000}"/>
+    <cellStyle name="Procentowy 3 3 3 2 2" xfId="920" xr:uid="{00000000-0005-0000-0000-000098030000}"/>
+    <cellStyle name="Procentowy 3 3 3 3" xfId="921" xr:uid="{00000000-0005-0000-0000-000099030000}"/>
+    <cellStyle name="Procentowy 3 3 4" xfId="922" xr:uid="{00000000-0005-0000-0000-00009A030000}"/>
+    <cellStyle name="Procentowy 3 3 4 2" xfId="923" xr:uid="{00000000-0005-0000-0000-00009B030000}"/>
+    <cellStyle name="Procentowy 3 3 5" xfId="924" xr:uid="{00000000-0005-0000-0000-00009C030000}"/>
+    <cellStyle name="Procentowy 3 4" xfId="925" xr:uid="{00000000-0005-0000-0000-00009D030000}"/>
+    <cellStyle name="Procentowy 3 4 2" xfId="926" xr:uid="{00000000-0005-0000-0000-00009E030000}"/>
+    <cellStyle name="Procentowy 3 4 2 2" xfId="927" xr:uid="{00000000-0005-0000-0000-00009F030000}"/>
+    <cellStyle name="Procentowy 3 4 2 2 2" xfId="928" xr:uid="{00000000-0005-0000-0000-0000A0030000}"/>
+    <cellStyle name="Procentowy 3 4 2 3" xfId="929" xr:uid="{00000000-0005-0000-0000-0000A1030000}"/>
+    <cellStyle name="Procentowy 3 4 3" xfId="930" xr:uid="{00000000-0005-0000-0000-0000A2030000}"/>
+    <cellStyle name="Procentowy 3 4 3 2" xfId="931" xr:uid="{00000000-0005-0000-0000-0000A3030000}"/>
+    <cellStyle name="Procentowy 3 4 4" xfId="932" xr:uid="{00000000-0005-0000-0000-0000A4030000}"/>
+    <cellStyle name="Procentowy 3 5" xfId="933" xr:uid="{00000000-0005-0000-0000-0000A5030000}"/>
+    <cellStyle name="Procentowy 3 5 2" xfId="934" xr:uid="{00000000-0005-0000-0000-0000A6030000}"/>
+    <cellStyle name="Procentowy 3 5 2 2" xfId="935" xr:uid="{00000000-0005-0000-0000-0000A7030000}"/>
+    <cellStyle name="Procentowy 3 5 3" xfId="936" xr:uid="{00000000-0005-0000-0000-0000A8030000}"/>
+    <cellStyle name="Procentowy 3 6" xfId="937" xr:uid="{00000000-0005-0000-0000-0000A9030000}"/>
+    <cellStyle name="Procentowy 3 6 2" xfId="938" xr:uid="{00000000-0005-0000-0000-0000AA030000}"/>
+    <cellStyle name="Procentowy 3 7" xfId="939" xr:uid="{00000000-0005-0000-0000-0000AB030000}"/>
+    <cellStyle name="Procentowy 4" xfId="940" xr:uid="{00000000-0005-0000-0000-0000AC030000}"/>
+    <cellStyle name="Procentowy 4 2" xfId="941" xr:uid="{00000000-0005-0000-0000-0000AD030000}"/>
+    <cellStyle name="Procentowy 4 3" xfId="942" xr:uid="{00000000-0005-0000-0000-0000AE030000}"/>
+    <cellStyle name="Procentowy 4 3 2" xfId="943" xr:uid="{00000000-0005-0000-0000-0000AF030000}"/>
+    <cellStyle name="Procentowy 4 3 2 2" xfId="944" xr:uid="{00000000-0005-0000-0000-0000B0030000}"/>
+    <cellStyle name="Procentowy 4 3 3" xfId="945" xr:uid="{00000000-0005-0000-0000-0000B1030000}"/>
+    <cellStyle name="Procentowy 4 4" xfId="946" xr:uid="{00000000-0005-0000-0000-0000B2030000}"/>
+    <cellStyle name="Procentowy 4 4 2" xfId="947" xr:uid="{00000000-0005-0000-0000-0000B3030000}"/>
+    <cellStyle name="Procentowy 4 5" xfId="948" xr:uid="{00000000-0005-0000-0000-0000B4030000}"/>
+    <cellStyle name="Procentowy 5" xfId="949" xr:uid="{00000000-0005-0000-0000-0000B5030000}"/>
+    <cellStyle name="Styl 1" xfId="950" xr:uid="{00000000-0005-0000-0000-0000B6030000}"/>
+    <cellStyle name="Uwaga 2" xfId="951" xr:uid="{00000000-0005-0000-0000-0000B7030000}"/>
+    <cellStyle name="Uwaga 2 2" xfId="952" xr:uid="{00000000-0005-0000-0000-0000B8030000}"/>
+    <cellStyle name="Uwaga 3" xfId="953" xr:uid="{00000000-0005-0000-0000-0000B9030000}"/>
+    <cellStyle name="Uwaga 3 2" xfId="954" xr:uid="{00000000-0005-0000-0000-0000BA030000}"/>
+    <cellStyle name="Walutowy 2" xfId="955" xr:uid="{00000000-0005-0000-0000-0000BB030000}"/>
+    <cellStyle name="Walutowy 2 2" xfId="956" xr:uid="{00000000-0005-0000-0000-0000BC030000}"/>
+    <cellStyle name="Walutowy 2 2 2" xfId="957" xr:uid="{00000000-0005-0000-0000-0000BD030000}"/>
+    <cellStyle name="Walutowy 2 3" xfId="958" xr:uid="{00000000-0005-0000-0000-0000BE030000}"/>
+    <cellStyle name="Walutowy 2 3 2" xfId="959" xr:uid="{00000000-0005-0000-0000-0000BF030000}"/>
+    <cellStyle name="Walutowy 2 3 2 2" xfId="960" xr:uid="{00000000-0005-0000-0000-0000C0030000}"/>
+    <cellStyle name="Walutowy 2 4" xfId="961" xr:uid="{00000000-0005-0000-0000-0000C1030000}"/>
+    <cellStyle name="Walutowy 2 5" xfId="962" xr:uid="{00000000-0005-0000-0000-0000C2030000}"/>
+    <cellStyle name="Walutowy 3" xfId="963" xr:uid="{00000000-0005-0000-0000-0000C3030000}"/>
+    <cellStyle name="Walutowy 3 2" xfId="964" xr:uid="{00000000-0005-0000-0000-0000C4030000}"/>
+    <cellStyle name="Walutowy 3 2 2" xfId="965" xr:uid="{00000000-0005-0000-0000-0000C5030000}"/>
+    <cellStyle name="Walutowy 3 2 2 2" xfId="966" xr:uid="{00000000-0005-0000-0000-0000C6030000}"/>
+    <cellStyle name="Walutowy 3 2 2 2 2" xfId="967" xr:uid="{00000000-0005-0000-0000-0000C7030000}"/>
+    <cellStyle name="Walutowy 3 2 2 2 2 2" xfId="968" xr:uid="{00000000-0005-0000-0000-0000C8030000}"/>
+    <cellStyle name="Walutowy 3 2 2 2 3" xfId="969" xr:uid="{00000000-0005-0000-0000-0000C9030000}"/>
+    <cellStyle name="Walutowy 3 2 2 3" xfId="970" xr:uid="{00000000-0005-0000-0000-0000CA030000}"/>
+    <cellStyle name="Walutowy 3 2 2 3 2" xfId="971" xr:uid="{00000000-0005-0000-0000-0000CB030000}"/>
+    <cellStyle name="Walutowy 3 2 2 4" xfId="972" xr:uid="{00000000-0005-0000-0000-0000CC030000}"/>
+    <cellStyle name="Walutowy 3 2 3" xfId="973" xr:uid="{00000000-0005-0000-0000-0000CD030000}"/>
+    <cellStyle name="Walutowy 3 2 3 2" xfId="974" xr:uid="{00000000-0005-0000-0000-0000CE030000}"/>
+    <cellStyle name="Walutowy 3 2 3 2 2" xfId="975" xr:uid="{00000000-0005-0000-0000-0000CF030000}"/>
+    <cellStyle name="Walutowy 3 2 3 3" xfId="976" xr:uid="{00000000-0005-0000-0000-0000D0030000}"/>
+    <cellStyle name="Walutowy 3 2 4" xfId="977" xr:uid="{00000000-0005-0000-0000-0000D1030000}"/>
+    <cellStyle name="Walutowy 3 2 4 2" xfId="978" xr:uid="{00000000-0005-0000-0000-0000D2030000}"/>
+    <cellStyle name="Walutowy 3 2 5" xfId="979" xr:uid="{00000000-0005-0000-0000-0000D3030000}"/>
+    <cellStyle name="Walutowy 3 3" xfId="980" xr:uid="{00000000-0005-0000-0000-0000D4030000}"/>
+    <cellStyle name="Walutowy 3 3 2" xfId="981" xr:uid="{00000000-0005-0000-0000-0000D5030000}"/>
+    <cellStyle name="Walutowy 3 3 2 2" xfId="982" xr:uid="{00000000-0005-0000-0000-0000D6030000}"/>
+    <cellStyle name="Walutowy 3 3 2 2 2" xfId="983" xr:uid="{00000000-0005-0000-0000-0000D7030000}"/>
+    <cellStyle name="Walutowy 3 3 2 2 2 2" xfId="984" xr:uid="{00000000-0005-0000-0000-0000D8030000}"/>
+    <cellStyle name="Walutowy 3 3 2 2 3" xfId="985" xr:uid="{00000000-0005-0000-0000-0000D9030000}"/>
+    <cellStyle name="Walutowy 3 3 2 3" xfId="986" xr:uid="{00000000-0005-0000-0000-0000DA030000}"/>
+    <cellStyle name="Walutowy 3 3 2 3 2" xfId="987" xr:uid="{00000000-0005-0000-0000-0000DB030000}"/>
+    <cellStyle name="Walutowy 3 3 2 4" xfId="988" xr:uid="{00000000-0005-0000-0000-0000DC030000}"/>
+    <cellStyle name="Walutowy 3 4" xfId="989" xr:uid="{00000000-0005-0000-0000-0000DD030000}"/>
+    <cellStyle name="Walutowy 3 4 2" xfId="990" xr:uid="{00000000-0005-0000-0000-0000DE030000}"/>
+    <cellStyle name="Walutowy 3 4 2 2" xfId="991" xr:uid="{00000000-0005-0000-0000-0000DF030000}"/>
+    <cellStyle name="Walutowy 3 4 3" xfId="992" xr:uid="{00000000-0005-0000-0000-0000E0030000}"/>
+    <cellStyle name="Walutowy 3 5" xfId="993" xr:uid="{00000000-0005-0000-0000-0000E1030000}"/>
+    <cellStyle name="Walutowy 3 5 2" xfId="994" xr:uid="{00000000-0005-0000-0000-0000E2030000}"/>
+    <cellStyle name="Walutowy 3 6" xfId="995" xr:uid="{00000000-0005-0000-0000-0000E3030000}"/>
+    <cellStyle name="Walutowy 4" xfId="996" xr:uid="{00000000-0005-0000-0000-0000E4030000}"/>
+    <cellStyle name="Walutowy 4 2" xfId="997" xr:uid="{00000000-0005-0000-0000-0000E5030000}"/>
+    <cellStyle name="Walutowy 4 2 2" xfId="998" xr:uid="{00000000-0005-0000-0000-0000E6030000}"/>
+    <cellStyle name="Walutowy 4 2 2 2" xfId="999" xr:uid="{00000000-0005-0000-0000-0000E7030000}"/>
+    <cellStyle name="Walutowy 4 2 2 2 2" xfId="1000" xr:uid="{00000000-0005-0000-0000-0000E8030000}"/>
+    <cellStyle name="Walutowy 4 2 2 2 2 2" xfId="1001" xr:uid="{00000000-0005-0000-0000-0000E9030000}"/>
+    <cellStyle name="Walutowy 4 2 2 2 3" xfId="1002" xr:uid="{00000000-0005-0000-0000-0000EA030000}"/>
+    <cellStyle name="Walutowy 4 2 2 3" xfId="1003" xr:uid="{00000000-0005-0000-0000-0000EB030000}"/>
+    <cellStyle name="Walutowy 4 2 2 3 2" xfId="1004" xr:uid="{00000000-0005-0000-0000-0000EC030000}"/>
+    <cellStyle name="Walutowy 4 2 2 4" xfId="1005" xr:uid="{00000000-0005-0000-0000-0000ED030000}"/>
+    <cellStyle name="Walutowy 4 2 3" xfId="1006" xr:uid="{00000000-0005-0000-0000-0000EE030000}"/>
+    <cellStyle name="Walutowy 4 2 3 2" xfId="1007" xr:uid="{00000000-0005-0000-0000-0000EF030000}"/>
+    <cellStyle name="Walutowy 4 2 3 2 2" xfId="1008" xr:uid="{00000000-0005-0000-0000-0000F0030000}"/>
+    <cellStyle name="Walutowy 4 2 3 3" xfId="1009" xr:uid="{00000000-0005-0000-0000-0000F1030000}"/>
+    <cellStyle name="Walutowy 4 2 4" xfId="1010" xr:uid="{00000000-0005-0000-0000-0000F2030000}"/>
+    <cellStyle name="Walutowy 4 2 4 2" xfId="1011" xr:uid="{00000000-0005-0000-0000-0000F3030000}"/>
+    <cellStyle name="Walutowy 4 2 5" xfId="1012" xr:uid="{00000000-0005-0000-0000-0000F4030000}"/>
+    <cellStyle name="Walutowy 4 3" xfId="1013" xr:uid="{00000000-0005-0000-0000-0000F5030000}"/>
+    <cellStyle name="Walutowy 4 3 2" xfId="1014" xr:uid="{00000000-0005-0000-0000-0000F6030000}"/>
+    <cellStyle name="Walutowy 4 3 2 2" xfId="1015" xr:uid="{00000000-0005-0000-0000-0000F7030000}"/>
+    <cellStyle name="Walutowy 4 3 2 2 2" xfId="1016" xr:uid="{00000000-0005-0000-0000-0000F8030000}"/>
+    <cellStyle name="Walutowy 4 3 2 3" xfId="1017" xr:uid="{00000000-0005-0000-0000-0000F9030000}"/>
+    <cellStyle name="Walutowy 4 3 3" xfId="1018" xr:uid="{00000000-0005-0000-0000-0000FA030000}"/>
+    <cellStyle name="Walutowy 4 3 3 2" xfId="1019" xr:uid="{00000000-0005-0000-0000-0000FB030000}"/>
+    <cellStyle name="Walutowy 4 3 4" xfId="1020" xr:uid="{00000000-0005-0000-0000-0000FC030000}"/>
+    <cellStyle name="Walutowy 4 4" xfId="1021" xr:uid="{00000000-0005-0000-0000-0000FD030000}"/>
+    <cellStyle name="Walutowy 4 4 2" xfId="1022" xr:uid="{00000000-0005-0000-0000-0000FE030000}"/>
+    <cellStyle name="Walutowy 4 4 2 2" xfId="1023" xr:uid="{00000000-0005-0000-0000-0000FF030000}"/>
+    <cellStyle name="Walutowy 4 4 3" xfId="1024" xr:uid="{00000000-0005-0000-0000-000000040000}"/>
+    <cellStyle name="Walutowy 4 5" xfId="1025" xr:uid="{00000000-0005-0000-0000-000001040000}"/>
+    <cellStyle name="Walutowy 4 5 2" xfId="1026" xr:uid="{00000000-0005-0000-0000-000002040000}"/>
+    <cellStyle name="Walutowy 4 6" xfId="1027" xr:uid="{00000000-0005-0000-0000-000003040000}"/>
+    <cellStyle name="Walutowy 5" xfId="1028" xr:uid="{00000000-0005-0000-0000-000004040000}"/>
+    <cellStyle name="Walutowy 5 2" xfId="1029" xr:uid="{00000000-0005-0000-0000-000005040000}"/>
+    <cellStyle name="Walutowy 5 2 2" xfId="1030" xr:uid="{00000000-0005-0000-0000-000006040000}"/>
+    <cellStyle name="Walutowy 5 2 2 2" xfId="1031" xr:uid="{00000000-0005-0000-0000-000007040000}"/>
+    <cellStyle name="Walutowy 5 2 2 2 2" xfId="1032" xr:uid="{00000000-0005-0000-0000-000008040000}"/>
+    <cellStyle name="Walutowy 5 2 2 2 2 2" xfId="1033" xr:uid="{00000000-0005-0000-0000-000009040000}"/>
+    <cellStyle name="Walutowy 5 2 2 2 3" xfId="1034" xr:uid="{00000000-0005-0000-0000-00000A040000}"/>
+    <cellStyle name="Walutowy 5 2 2 3" xfId="1035" xr:uid="{00000000-0005-0000-0000-00000B040000}"/>
+    <cellStyle name="Walutowy 5 2 2 3 2" xfId="1036" xr:uid="{00000000-0005-0000-0000-00000C040000}"/>
+    <cellStyle name="Walutowy 5 2 2 4" xfId="1037" xr:uid="{00000000-0005-0000-0000-00000D040000}"/>
+    <cellStyle name="Walutowy 5 2 3" xfId="1038" xr:uid="{00000000-0005-0000-0000-00000E040000}"/>
+    <cellStyle name="Walutowy 5 2 3 2" xfId="1039" xr:uid="{00000000-0005-0000-0000-00000F040000}"/>
+    <cellStyle name="Walutowy 5 2 3 2 2" xfId="1040" xr:uid="{00000000-0005-0000-0000-000010040000}"/>
+    <cellStyle name="Walutowy 5 2 3 3" xfId="1041" xr:uid="{00000000-0005-0000-0000-000011040000}"/>
+    <cellStyle name="Walutowy 5 2 4" xfId="1042" xr:uid="{00000000-0005-0000-0000-000012040000}"/>
+    <cellStyle name="Walutowy 5 2 4 2" xfId="1043" xr:uid="{00000000-0005-0000-0000-000013040000}"/>
+    <cellStyle name="Walutowy 5 2 5" xfId="1044" xr:uid="{00000000-0005-0000-0000-000014040000}"/>
+    <cellStyle name="Walutowy 5 3" xfId="1045" xr:uid="{00000000-0005-0000-0000-000015040000}"/>
+    <cellStyle name="Walutowy 5 3 2" xfId="1046" xr:uid="{00000000-0005-0000-0000-000016040000}"/>
+    <cellStyle name="Walutowy 5 3 2 2" xfId="1047" xr:uid="{00000000-0005-0000-0000-000017040000}"/>
+    <cellStyle name="Walutowy 5 3 2 2 2" xfId="1048" xr:uid="{00000000-0005-0000-0000-000018040000}"/>
+    <cellStyle name="Walutowy 5 3 2 3" xfId="1049" xr:uid="{00000000-0005-0000-0000-000019040000}"/>
+    <cellStyle name="Walutowy 5 3 3" xfId="1050" xr:uid="{00000000-0005-0000-0000-00001A040000}"/>
+    <cellStyle name="Walutowy 5 3 3 2" xfId="1051" xr:uid="{00000000-0005-0000-0000-00001B040000}"/>
+    <cellStyle name="Walutowy 5 3 4" xfId="1052" xr:uid="{00000000-0005-0000-0000-00001C040000}"/>
+    <cellStyle name="Walutowy 5 4" xfId="1053" xr:uid="{00000000-0005-0000-0000-00001D040000}"/>
+    <cellStyle name="Walutowy 5 4 2" xfId="1054" xr:uid="{00000000-0005-0000-0000-00001E040000}"/>
+    <cellStyle name="Walutowy 5 4 2 2" xfId="1055" xr:uid="{00000000-0005-0000-0000-00001F040000}"/>
+    <cellStyle name="Walutowy 5 4 3" xfId="1056" xr:uid="{00000000-0005-0000-0000-000020040000}"/>
+    <cellStyle name="Walutowy 5 5" xfId="1057" xr:uid="{00000000-0005-0000-0000-000021040000}"/>
+    <cellStyle name="Walutowy 5 5 2" xfId="1058" xr:uid="{00000000-0005-0000-0000-000022040000}"/>
+    <cellStyle name="Walutowy 5 6" xfId="1059" xr:uid="{00000000-0005-0000-0000-000023040000}"/>
+    <cellStyle name="Walutowy 6" xfId="1060" xr:uid="{00000000-0005-0000-0000-000024040000}"/>
+    <cellStyle name="Walutowy 6 2" xfId="1061" xr:uid="{00000000-0005-0000-0000-000025040000}"/>
+    <cellStyle name="Walutowy 6 2 2" xfId="1062" xr:uid="{00000000-0005-0000-0000-000026040000}"/>
+    <cellStyle name="Walutowy 6 2 2 2" xfId="1063" xr:uid="{00000000-0005-0000-0000-000027040000}"/>
+    <cellStyle name="Walutowy 6 2 2 2 2" xfId="1064" xr:uid="{00000000-0005-0000-0000-000028040000}"/>
+    <cellStyle name="Walutowy 6 2 2 2 2 2" xfId="1065" xr:uid="{00000000-0005-0000-0000-000029040000}"/>
+    <cellStyle name="Walutowy 6 2 2 2 3" xfId="1066" xr:uid="{00000000-0005-0000-0000-00002A040000}"/>
+    <cellStyle name="Walutowy 6 2 2 3" xfId="1067" xr:uid="{00000000-0005-0000-0000-00002B040000}"/>
+    <cellStyle name="Walutowy 6 2 2 3 2" xfId="1068" xr:uid="{00000000-0005-0000-0000-00002C040000}"/>
+    <cellStyle name="Walutowy 6 2 2 4" xfId="1069" xr:uid="{00000000-0005-0000-0000-00002D040000}"/>
+    <cellStyle name="Walutowy 6 2 3" xfId="1070" xr:uid="{00000000-0005-0000-0000-00002E040000}"/>
+    <cellStyle name="Walutowy 6 2 3 2" xfId="1071" xr:uid="{00000000-0005-0000-0000-00002F040000}"/>
+    <cellStyle name="Walutowy 6 2 3 2 2" xfId="1072" xr:uid="{00000000-0005-0000-0000-000030040000}"/>
+    <cellStyle name="Walutowy 6 2 3 3" xfId="1073" xr:uid="{00000000-0005-0000-0000-000031040000}"/>
+    <cellStyle name="Walutowy 6 2 4" xfId="1074" xr:uid="{00000000-0005-0000-0000-000032040000}"/>
+    <cellStyle name="Walutowy 6 2 4 2" xfId="1075" xr:uid="{00000000-0005-0000-0000-000033040000}"/>
+    <cellStyle name="Walutowy 6 2 5" xfId="1076" xr:uid="{00000000-0005-0000-0000-000034040000}"/>
+    <cellStyle name="Walutowy 6 3" xfId="1077" xr:uid="{00000000-0005-0000-0000-000035040000}"/>
+    <cellStyle name="Walutowy 6 3 2" xfId="1078" xr:uid="{00000000-0005-0000-0000-000036040000}"/>
+    <cellStyle name="Walutowy 6 3 2 2" xfId="1079" xr:uid="{00000000-0005-0000-0000-000037040000}"/>
+    <cellStyle name="Walutowy 6 3 2 2 2" xfId="1080" xr:uid="{00000000-0005-0000-0000-000038040000}"/>
+    <cellStyle name="Walutowy 6 3 2 3" xfId="1081" xr:uid="{00000000-0005-0000-0000-000039040000}"/>
+    <cellStyle name="Walutowy 6 3 3" xfId="1082" xr:uid="{00000000-0005-0000-0000-00003A040000}"/>
+    <cellStyle name="Walutowy 6 3 3 2" xfId="1083" xr:uid="{00000000-0005-0000-0000-00003B040000}"/>
+    <cellStyle name="Walutowy 6 3 4" xfId="1084" xr:uid="{00000000-0005-0000-0000-00003C040000}"/>
+    <cellStyle name="Walutowy 6 4" xfId="1085" xr:uid="{00000000-0005-0000-0000-00003D040000}"/>
+    <cellStyle name="Walutowy 6 4 2" xfId="1086" xr:uid="{00000000-0005-0000-0000-00003E040000}"/>
+    <cellStyle name="Walutowy 6 4 2 2" xfId="1087" xr:uid="{00000000-0005-0000-0000-00003F040000}"/>
+    <cellStyle name="Walutowy 6 4 3" xfId="1088" xr:uid="{00000000-0005-0000-0000-000040040000}"/>
+    <cellStyle name="Walutowy 6 5" xfId="1089" xr:uid="{00000000-0005-0000-0000-000041040000}"/>
+    <cellStyle name="Walutowy 6 5 2" xfId="1090" xr:uid="{00000000-0005-0000-0000-000042040000}"/>
+    <cellStyle name="Walutowy 6 6" xfId="1091" xr:uid="{00000000-0005-0000-0000-000043040000}"/>
+    <cellStyle name="Walutowy 7" xfId="1092" xr:uid="{00000000-0005-0000-0000-000044040000}"/>
+    <cellStyle name="Walutowy 7 2" xfId="1093" xr:uid="{00000000-0005-0000-0000-000045040000}"/>
+    <cellStyle name="Walutowy 7 2 2" xfId="1094" xr:uid="{00000000-0005-0000-0000-000046040000}"/>
+    <cellStyle name="Walutowy 7 2 2 2" xfId="1095" xr:uid="{00000000-0005-0000-0000-000047040000}"/>
+    <cellStyle name="Walutowy 7 2 3" xfId="1096" xr:uid="{00000000-0005-0000-0000-000048040000}"/>
+    <cellStyle name="Walutowy 7 3" xfId="1097" xr:uid="{00000000-0005-0000-0000-000049040000}"/>
+    <cellStyle name="Walutowy 7 3 2" xfId="1098" xr:uid="{00000000-0005-0000-0000-00004A040000}"/>
+    <cellStyle name="Walutowy 7 4" xfId="1099" xr:uid="{00000000-0005-0000-0000-00004B040000}"/>
+    <cellStyle name="Walutowy 8" xfId="1100" xr:uid="{00000000-0005-0000-0000-00004C040000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3544,7 +3551,7 @@
         <xdr:cNvPr id="7" name="Obraz 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3556,7 +3563,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3576,7 +3583,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3605,7 +3612,7 @@
         <xdr:cNvPr id="2" name="Skos 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3682,7 +3689,7 @@
         <xdr:cNvPr id="5" name="Skos 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3739,44 +3746,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>329713</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>23644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95252</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>194161</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Obraz 5" descr="pieczątka M.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1018444" y="8508221"/>
-          <a:ext cx="1890346" cy="859248"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>102578</xdr:colOff>
       <xdr:row>37</xdr:row>
@@ -3790,13 +3759,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Obraz 7" descr="pieczątka MP.jpg"/>
+        <xdr:cNvPr id="8" name="Obraz 7" descr="pieczątka MP.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3805,6 +3780,104 @@
         <a:xfrm>
           <a:off x="4308232" y="8562132"/>
           <a:ext cx="1619250" cy="773100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>666750</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>339586</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>729060</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>94332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2715052-08BE-4E67-BAC4-2E0EC8C159AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1027043" y="8531087"/>
+          <a:ext cx="1780952" cy="723810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3859,7 +3932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3891,9 +3964,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3925,6 +4016,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -4100,28 +4209,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A23" zoomScale="115" zoomScaleNormal="70" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="4" max="4" width="9.375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="14.4" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="36.6" thickBot="1">
+    <row r="3" spans="1:9" ht="36.75" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
@@ -4151,44 +4260,44 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="48.75" customHeight="1">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="60">
         <v>9075</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="83">
+      <c r="H4" s="60">
         <v>779</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="60" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="86"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4"/>
@@ -4217,7 +4326,7 @@
     <row r="14" spans="1:9">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="19.8" thickBot="1">
+    <row r="15" spans="1:9" ht="18.75" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>3</v>
       </c>
@@ -4246,7 +4355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19.2">
+    <row r="16" spans="1:9" ht="18">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -4276,24 +4385,24 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76" t="s">
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="76" t="s">
+      <c r="G17" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="70" t="s">
+      <c r="H17" s="64" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="66" t="s">
@@ -4301,17 +4410,17 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="71"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="65"/>
       <c r="I18" s="66"/>
     </row>
-    <row r="19" spans="1:9" ht="19.2">
+    <row r="19" spans="1:9" ht="18">
       <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
@@ -4327,117 +4436,117 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55" t="s">
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
     </row>
-    <row r="22" spans="1:9" ht="14.4" thickBot="1">
-      <c r="A22" s="73"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
+    <row r="22" spans="1:9" ht="15" thickBot="1">
+      <c r="A22" s="68"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53" t="s">
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
     </row>
-    <row r="24" spans="1:9" ht="20.399999999999999">
+    <row r="24" spans="1:9" ht="22.5">
       <c r="A24" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
       <c r="F24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="14.4" thickBot="1">
+    <row r="26" spans="1:9" ht="15" thickBot="1">
       <c r="A26" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57" t="s">
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69" t="s">
+      <c r="C27" s="75"/>
+      <c r="D27" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="76" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="66"/>
@@ -4445,27 +4554,27 @@
         <v>32</v>
       </c>
       <c r="E28" s="66"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="65"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="66" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="66"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
     </row>
     <row r="30" spans="1:9" ht="22.5" customHeight="1">
       <c r="A30" s="30" t="s">
@@ -4479,16 +4588,16 @@
         <v>37</v>
       </c>
       <c r="E30" s="66"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
     </row>
-    <row r="31" spans="1:9" ht="20.399999999999999">
+    <row r="31" spans="1:9" ht="22.5">
       <c r="A31" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="76" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="66"/>
@@ -4496,10 +4605,10 @@
         <v>40</v>
       </c>
       <c r="E31" s="66"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="29" t="s">
@@ -4517,12 +4626,12 @@
       <c r="E32" s="14">
         <v>2.5</v>
       </c>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -4530,65 +4639,65 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:9" ht="14.4" thickBot="1">
+    <row r="34" spans="1:9" ht="15" thickBot="1">
       <c r="A34" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61" t="s">
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
     </row>
     <row r="35" spans="1:9" ht="26.25" customHeight="1" thickBot="1">
       <c r="A35" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79" t="s">
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="80"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="57"/>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A37" s="77" t="s">
+      <c r="A37" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78" t="s">
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="81"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="1:9" ht="27" customHeight="1">
       <c r="A38" s="35"/>
@@ -4613,24 +4722,24 @@
       <c r="I39" s="48"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1">
-      <c r="A40" s="87"/>
+      <c r="A40" s="52"/>
       <c r="B40" s="51"/>
       <c r="C40" s="41"/>
       <c r="D40" s="41"/>
       <c r="E40" s="42"/>
-      <c r="F40" s="88"/>
+      <c r="F40" s="53"/>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
       <c r="I40" s="50"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="13"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -4639,6 +4748,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B21:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F21:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="F36:I36"/>
     <mergeCell ref="F37:I37"/>
@@ -4655,37 +4795,6 @@
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B21:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F21:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
@@ -4700,20 +4809,44 @@
   <legacyDrawing r:id="rId3"/>
   <legacyDrawingHF r:id="rId4"/>
   <oleObjects>
-    <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>666750</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>